<commit_message>
- CRMF2080: Bổ sung trường Loại yêu cầu - CRMF2081: Bổ sung trường: Loại yêu cầu, Phân loại bug, Chủ đề yêu cầu, Dự án, Deadline mong muốn, Deadline xử lý, Deadline thực tế, Số giờ cho phép, Số giờ thực tế - CRMF2082: Bổ sung các trường: Loại yêu cầu, Dự án, Deadline mong muốn, Deadline thực tế hoàn thành, Số giờ cho phép, Số giờ thực tế,
</commit_message>
<xml_diff>
--- a/2018/CRM/03_DetailDesign/CRMF2080_Danh muc yeu cau.xlsx
+++ b/2018/CRM/03_DetailDesign/CRMF2080_Danh muc yeu cau.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ASOFT_ERP9\10_DOCUMENT\13_DETAIL_DESIGN\1.STANDARD\ASOFT_CRM\03_DetailDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01.CRM\1_Tài liệu phân tích_Yêu cầu\03_DetailDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Coverpage" sheetId="20" r:id="rId1"/>
@@ -1333,7 +1333,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="331">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2348,38 +2348,6 @@
     <t>- Sự kiện click button [btnPrint] lấy danh sách APKlist search từ @SQL008 được gọi đến màn hình in CRMR20801</t>
   </si>
   <si>
-    <t xml:space="preserve">EXEC CRMP20803 ( 
-  @DivisionID VARCHAR(50),  
-  @DivisionIDList NVARCHAR(2000),     
-  @RequestSubject nvarchar(50),
-  @AccountID nvarchar(250),
-  @AssignedToUserID nvarchar(250),
-  @RequestStatus nvarchar(250),
-  @PriorityID nvarchar(100),
-  @UserID  VARCHAR(50)
-) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   @DivisionID   
-  @DivisionIDList      
-  @RequestSubject 
-  @AccountID 
-  @AssignedToUserID 
-  @RequestStatus 
-  @PriorityID 
-  @UserID  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Biến môi trường   
-  @DivisionIDList      
-  @RequestSubject 
-  @AccountID 
-  @AssignedToUserID 
-  @RequestStatus 
-  @PriorityID 
-  Biến môi trường  </t>
-  </si>
-  <si>
     <t>AccountID</t>
   </si>
   <si>
@@ -2551,6 +2519,27 @@
     </r>
   </si>
   <si>
+    <t>Bổ sung phân quyền @ConditionRequestID</t>
+  </si>
+  <si>
+    <t>Tấn Đạt</t>
+  </si>
+  <si>
+    <t>26/01/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bổ sung trường Loại yêu cầu </t>
+  </si>
+  <si>
+    <t>Loại yêu cầu</t>
+  </si>
+  <si>
+    <t>RequestTypeID</t>
+  </si>
+  <si>
+    <t>Ver 2.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">EXEC CRMP20801 ( 
   @DivisionID VARCHAR(50),  
   @DivisionIDList NVARCHAR(2000),     
@@ -2562,7 +2551,8 @@
   @UserID  VARCHAR(50),
   @ConditionRequestID Nvarchar(max), 
   @PageNumber INT,
-  @PageSize INT
+  @PageSize INT,
+  @RequestTypeID
 ) </t>
   </si>
   <si>
@@ -2576,7 +2566,8 @@
   @UserID  
 @ConditionRequestID
   @PageNumber 
-  @PageSize </t>
+  @PageSize 
+  @RequestTypeID</t>
   </si>
   <si>
     <t xml:space="preserve"> Biến môi trường   
@@ -2589,10 +2580,54 @@
   Biến môi trường 
 @ConditionRequestID 
   @PageNumber 
-  @PageSize </t>
-  </si>
-  <si>
-    <t>Bổ sung phân quyền @ConditionRequestID</t>
+  @PageSize 
+  @RequestTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXEC CRMP20803 ( 
+  @DivisionID VARCHAR(50),  
+  @DivisionIDList NVARCHAR(2000),     
+  @RequestSubject nvarchar(50),
+  @AccountID nvarchar(250),
+  @AssignedToUserID nvarchar(250),
+  @RequestStatus nvarchar(250),
+  @PriorityID nvarchar(100),
+  @UserID  VARCHAR(50),
+  @RequestTypeID nvarchar(250)
+) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   @DivisionID   
+  @DivisionIDList      
+  @RequestSubject 
+  @AccountID 
+  @AssignedToUserID 
+  @RequestStatus 
+  @PriorityID 
+  @UserID 
+  @RequestTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Biến môi trường   
+  @DivisionIDList      
+  @RequestSubject 
+  @AccountID 
+  @AssignedToUserID 
+  @RequestStatus 
+  @PriorityID 
+  Biến môi trường  
+  @RequestTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   @DivisionID   
+  @DivisionIDList      
+  @RequestSubject 
+  @AccountID 
+  @AssignedToUserID 
+  @RequestStatus 
+  @PriorityID 
+  @UserID  
+  @RequestTypeID</t>
   </si>
 </sst>
 </file>
@@ -3116,7 +3151,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3444,9 +3479,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3490,9 +3522,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3505,75 +3534,90 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3592,21 +3636,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3694,6 +3723,27 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3703,24 +3753,6 @@
     <xf numFmtId="14" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3730,27 +3762,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3774,6 +3785,61 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -3791,6 +3857,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF00FF"/>
       <color rgb="FF00FFFF"/>
     </mruColors>
   </colors>
@@ -3861,15 +3928,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2533650</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3893,8 +3960,63 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="161925" y="876300"/>
+          <a:off x="47625" y="800100"/>
           <a:ext cx="9639300" cy="5800725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2543175</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="762000"/>
+          <a:ext cx="9696450" cy="5867400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4748,65 +4870,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1">
-      <c r="A1" s="165"/>
-      <c r="B1" s="165"/>
-      <c r="C1" s="167" t="s">
+      <c r="A1" s="157"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="159" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
-      <c r="F1" s="169"/>
-      <c r="G1" s="166" t="s">
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="158" t="s">
         <v>148</v>
       </c>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166" t="s">
+      <c r="H1" s="158"/>
+      <c r="I1" s="158" t="s">
         <v>149</v>
       </c>
-      <c r="J1" s="166"/>
+      <c r="J1" s="158"/>
     </row>
     <row r="2" spans="1:18" ht="23.25" customHeight="1">
-      <c r="A2" s="165"/>
-      <c r="B2" s="165"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="172"/>
-      <c r="G2" s="166" t="s">
+      <c r="A2" s="157"/>
+      <c r="B2" s="157"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="158" t="s">
         <v>150</v>
       </c>
-      <c r="H2" s="166"/>
-      <c r="I2" s="166"/>
-      <c r="J2" s="166"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
     </row>
     <row r="3" spans="1:18" ht="12.75" customHeight="1">
-      <c r="A3" s="165"/>
-      <c r="B3" s="165"/>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="162" t="s">
+      <c r="A3" s="157"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="154" t="s">
         <v>151</v>
       </c>
-      <c r="H3" s="163"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="163"/>
+      <c r="H3" s="155"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="155"/>
     </row>
     <row r="4" spans="1:18">
       <c r="H4" s="98"/>
     </row>
     <row r="13" spans="1:18" ht="30">
-      <c r="A13" s="164"/>
-      <c r="B13" s="164"/>
-      <c r="C13" s="164"/>
-      <c r="D13" s="164"/>
-      <c r="E13" s="164"/>
-      <c r="F13" s="164"/>
-      <c r="G13" s="164"/>
-      <c r="H13" s="164"/>
-      <c r="I13" s="164"/>
-      <c r="J13" s="164"/>
+      <c r="A13" s="156"/>
+      <c r="B13" s="156"/>
+      <c r="C13" s="156"/>
+      <c r="D13" s="156"/>
+      <c r="E13" s="156"/>
+      <c r="F13" s="156"/>
+      <c r="G13" s="156"/>
+      <c r="H13" s="156"/>
+      <c r="I13" s="156"/>
+      <c r="J13" s="156"/>
       <c r="K13" s="99"/>
       <c r="L13" s="99"/>
       <c r="M13" s="99"/>
@@ -4817,56 +4939,56 @@
       <c r="R13" s="99"/>
     </row>
     <row r="14" spans="1:18" ht="26.25">
-      <c r="B14" s="158"/>
-      <c r="C14" s="158"/>
-      <c r="D14" s="158"/>
-      <c r="E14" s="158"/>
-      <c r="F14" s="158"/>
-      <c r="G14" s="158"/>
-      <c r="H14" s="158"/>
-      <c r="I14" s="158"/>
-      <c r="J14" s="158"/>
-      <c r="K14" s="158"/>
-      <c r="L14" s="158"/>
-      <c r="M14" s="158"/>
-      <c r="N14" s="158"/>
-      <c r="O14" s="158"/>
-      <c r="P14" s="158"/>
-      <c r="Q14" s="158"/>
-      <c r="R14" s="158"/>
+      <c r="B14" s="152"/>
+      <c r="C14" s="152"/>
+      <c r="D14" s="152"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="152"/>
+      <c r="H14" s="152"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="152"/>
+      <c r="K14" s="152"/>
+      <c r="L14" s="152"/>
+      <c r="M14" s="152"/>
+      <c r="N14" s="152"/>
+      <c r="O14" s="152"/>
+      <c r="P14" s="152"/>
+      <c r="Q14" s="152"/>
+      <c r="R14" s="152"/>
     </row>
     <row r="15" spans="1:18" ht="26.25">
-      <c r="B15" s="158"/>
-      <c r="C15" s="158"/>
-      <c r="D15" s="158"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
-      <c r="K15" s="158"/>
-      <c r="L15" s="158"/>
-      <c r="M15" s="158"/>
-      <c r="N15" s="158"/>
-      <c r="O15" s="158"/>
-      <c r="P15" s="158"/>
-      <c r="Q15" s="158"/>
-      <c r="R15" s="158"/>
+      <c r="B15" s="152"/>
+      <c r="C15" s="152"/>
+      <c r="D15" s="152"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
+      <c r="L15" s="152"/>
+      <c r="M15" s="152"/>
+      <c r="N15" s="152"/>
+      <c r="O15" s="152"/>
+      <c r="P15" s="152"/>
+      <c r="Q15" s="152"/>
+      <c r="R15" s="152"/>
     </row>
     <row r="16" spans="1:18" ht="26.25">
-      <c r="A16" s="161" t="s">
+      <c r="A16" s="153" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="161"/>
-      <c r="C16" s="161"/>
-      <c r="D16" s="161"/>
-      <c r="E16" s="161"/>
-      <c r="F16" s="161"/>
-      <c r="G16" s="161"/>
-      <c r="H16" s="161"/>
-      <c r="I16" s="161"/>
-      <c r="J16" s="161"/>
+      <c r="B16" s="153"/>
+      <c r="C16" s="153"/>
+      <c r="D16" s="153"/>
+      <c r="E16" s="153"/>
+      <c r="F16" s="153"/>
+      <c r="G16" s="153"/>
+      <c r="H16" s="153"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="153"/>
       <c r="K16" s="100"/>
       <c r="L16" s="100"/>
       <c r="M16" s="100"/>
@@ -4877,384 +4999,384 @@
       <c r="R16" s="100"/>
     </row>
     <row r="17" spans="1:195" ht="14.1" customHeight="1">
-      <c r="B17" s="158"/>
-      <c r="C17" s="158"/>
-      <c r="D17" s="158"/>
-      <c r="E17" s="158"/>
-      <c r="F17" s="158"/>
-      <c r="G17" s="158"/>
-      <c r="H17" s="158"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="158"/>
-      <c r="K17" s="158"/>
-      <c r="L17" s="158"/>
-      <c r="M17" s="158"/>
-      <c r="N17" s="158"/>
-      <c r="O17" s="158"/>
-      <c r="P17" s="158"/>
-      <c r="Q17" s="158"/>
-      <c r="R17" s="158"/>
+      <c r="B17" s="152"/>
+      <c r="C17" s="152"/>
+      <c r="D17" s="152"/>
+      <c r="E17" s="152"/>
+      <c r="F17" s="152"/>
+      <c r="G17" s="152"/>
+      <c r="H17" s="152"/>
+      <c r="I17" s="152"/>
+      <c r="J17" s="152"/>
+      <c r="K17" s="152"/>
+      <c r="L17" s="152"/>
+      <c r="M17" s="152"/>
+      <c r="N17" s="152"/>
+      <c r="O17" s="152"/>
+      <c r="P17" s="152"/>
+      <c r="Q17" s="152"/>
+      <c r="R17" s="152"/>
     </row>
     <row r="18" spans="1:195" ht="26.25">
-      <c r="B18" s="158"/>
-      <c r="C18" s="158"/>
-      <c r="D18" s="158"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
-      <c r="K18" s="158"/>
-      <c r="L18" s="158"/>
-      <c r="M18" s="158"/>
-      <c r="N18" s="158"/>
-      <c r="O18" s="158"/>
-      <c r="P18" s="158"/>
-      <c r="Q18" s="158"/>
-      <c r="R18" s="158"/>
+      <c r="B18" s="152"/>
+      <c r="C18" s="152"/>
+      <c r="D18" s="152"/>
+      <c r="E18" s="152"/>
+      <c r="F18" s="152"/>
+      <c r="G18" s="152"/>
+      <c r="H18" s="152"/>
+      <c r="I18" s="152"/>
+      <c r="J18" s="152"/>
+      <c r="K18" s="152"/>
+      <c r="L18" s="152"/>
+      <c r="M18" s="152"/>
+      <c r="N18" s="152"/>
+      <c r="O18" s="152"/>
+      <c r="P18" s="152"/>
+      <c r="Q18" s="152"/>
+      <c r="R18" s="152"/>
     </row>
     <row r="19" spans="1:195" ht="23.25">
-      <c r="B19" s="160"/>
-      <c r="C19" s="160"/>
-      <c r="D19" s="160"/>
-      <c r="E19" s="160"/>
-      <c r="F19" s="160"/>
-      <c r="G19" s="160"/>
-      <c r="H19" s="160"/>
-      <c r="I19" s="160"/>
-      <c r="J19" s="160"/>
-      <c r="K19" s="160"/>
-      <c r="L19" s="160"/>
-      <c r="M19" s="160"/>
-      <c r="N19" s="160"/>
-      <c r="O19" s="160"/>
-      <c r="P19" s="160"/>
-      <c r="Q19" s="160"/>
-      <c r="R19" s="160"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="169"/>
+      <c r="D19" s="169"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="169"/>
+      <c r="G19" s="169"/>
+      <c r="H19" s="169"/>
+      <c r="I19" s="169"/>
+      <c r="J19" s="169"/>
+      <c r="K19" s="169"/>
+      <c r="L19" s="169"/>
+      <c r="M19" s="169"/>
+      <c r="N19" s="169"/>
+      <c r="O19" s="169"/>
+      <c r="P19" s="169"/>
+      <c r="Q19" s="169"/>
+      <c r="R19" s="169"/>
     </row>
     <row r="20" spans="1:195" ht="26.25">
-      <c r="B20" s="158"/>
-      <c r="C20" s="158"/>
-      <c r="D20" s="158"/>
-      <c r="E20" s="158"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158"/>
-      <c r="J20" s="158"/>
-      <c r="K20" s="158"/>
-      <c r="L20" s="158"/>
-      <c r="M20" s="158"/>
-      <c r="N20" s="158"/>
-      <c r="O20" s="158"/>
-      <c r="P20" s="158"/>
-      <c r="Q20" s="158"/>
-      <c r="R20" s="158"/>
+      <c r="B20" s="152"/>
+      <c r="C20" s="152"/>
+      <c r="D20" s="152"/>
+      <c r="E20" s="152"/>
+      <c r="F20" s="152"/>
+      <c r="G20" s="152"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="152"/>
+      <c r="J20" s="152"/>
+      <c r="K20" s="152"/>
+      <c r="L20" s="152"/>
+      <c r="M20" s="152"/>
+      <c r="N20" s="152"/>
+      <c r="O20" s="152"/>
+      <c r="P20" s="152"/>
+      <c r="Q20" s="152"/>
+      <c r="R20" s="152"/>
     </row>
     <row r="21" spans="1:195" ht="26.25">
-      <c r="B21" s="158"/>
-      <c r="C21" s="158"/>
-      <c r="D21" s="158"/>
-      <c r="E21" s="158"/>
-      <c r="F21" s="158"/>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158"/>
-      <c r="J21" s="158"/>
-      <c r="K21" s="158"/>
-      <c r="L21" s="158"/>
-      <c r="M21" s="158"/>
-      <c r="N21" s="158"/>
-      <c r="O21" s="158"/>
-      <c r="P21" s="158"/>
-      <c r="Q21" s="158"/>
-      <c r="R21" s="158"/>
+      <c r="B21" s="152"/>
+      <c r="C21" s="152"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="152"/>
+      <c r="G21" s="152"/>
+      <c r="H21" s="152"/>
+      <c r="I21" s="152"/>
+      <c r="J21" s="152"/>
+      <c r="K21" s="152"/>
+      <c r="L21" s="152"/>
+      <c r="M21" s="152"/>
+      <c r="N21" s="152"/>
+      <c r="O21" s="152"/>
+      <c r="P21" s="152"/>
+      <c r="Q21" s="152"/>
+      <c r="R21" s="152"/>
     </row>
     <row r="22" spans="1:195" ht="25.5">
-      <c r="B22" s="159"/>
-      <c r="C22" s="159"/>
-      <c r="D22" s="159"/>
-      <c r="E22" s="159"/>
-      <c r="F22" s="159"/>
-      <c r="G22" s="159"/>
-      <c r="H22" s="159"/>
-      <c r="I22" s="159"/>
-      <c r="J22" s="159"/>
-      <c r="K22" s="159"/>
-      <c r="L22" s="159"/>
-      <c r="M22" s="159"/>
-      <c r="N22" s="159"/>
-      <c r="O22" s="159"/>
-      <c r="P22" s="159"/>
-      <c r="Q22" s="159"/>
-      <c r="R22" s="159"/>
+      <c r="B22" s="168"/>
+      <c r="C22" s="168"/>
+      <c r="D22" s="168"/>
+      <c r="E22" s="168"/>
+      <c r="F22" s="168"/>
+      <c r="G22" s="168"/>
+      <c r="H22" s="168"/>
+      <c r="I22" s="168"/>
+      <c r="J22" s="168"/>
+      <c r="K22" s="168"/>
+      <c r="L22" s="168"/>
+      <c r="M22" s="168"/>
+      <c r="N22" s="168"/>
+      <c r="O22" s="168"/>
+      <c r="P22" s="168"/>
+      <c r="Q22" s="168"/>
+      <c r="R22" s="168"/>
     </row>
     <row r="23" spans="1:195" ht="25.5">
-      <c r="B23" s="159"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="159"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="159"/>
-      <c r="H23" s="159"/>
-      <c r="I23" s="159"/>
-      <c r="J23" s="159"/>
-      <c r="K23" s="159"/>
-      <c r="L23" s="159"/>
-      <c r="M23" s="159"/>
-      <c r="N23" s="159"/>
-      <c r="O23" s="159"/>
-      <c r="P23" s="159"/>
-      <c r="Q23" s="159"/>
-      <c r="R23" s="159"/>
+      <c r="B23" s="168"/>
+      <c r="C23" s="168"/>
+      <c r="D23" s="168"/>
+      <c r="E23" s="168"/>
+      <c r="F23" s="168"/>
+      <c r="G23" s="168"/>
+      <c r="H23" s="168"/>
+      <c r="I23" s="168"/>
+      <c r="J23" s="168"/>
+      <c r="K23" s="168"/>
+      <c r="L23" s="168"/>
+      <c r="M23" s="168"/>
+      <c r="N23" s="168"/>
+      <c r="O23" s="168"/>
+      <c r="P23" s="168"/>
+      <c r="Q23" s="168"/>
+      <c r="R23" s="168"/>
     </row>
     <row r="25" spans="1:195" ht="11.25" customHeight="1"/>
     <row r="26" spans="1:195" ht="18">
-      <c r="B26" s="156"/>
-      <c r="C26" s="156"/>
-      <c r="D26" s="156"/>
-      <c r="E26" s="156"/>
-      <c r="F26" s="156"/>
-      <c r="G26" s="156"/>
-      <c r="H26" s="156"/>
-      <c r="I26" s="156"/>
-      <c r="J26" s="156"/>
-      <c r="K26" s="156"/>
-      <c r="L26" s="156"/>
-      <c r="M26" s="156"/>
-      <c r="N26" s="156"/>
-      <c r="O26" s="156"/>
-      <c r="P26" s="156"/>
-      <c r="Q26" s="156"/>
-      <c r="R26" s="156"/>
+      <c r="B26" s="170"/>
+      <c r="C26" s="170"/>
+      <c r="D26" s="170"/>
+      <c r="E26" s="170"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="170"/>
+      <c r="H26" s="170"/>
+      <c r="I26" s="170"/>
+      <c r="J26" s="170"/>
+      <c r="K26" s="170"/>
+      <c r="L26" s="170"/>
+      <c r="M26" s="170"/>
+      <c r="N26" s="170"/>
+      <c r="O26" s="170"/>
+      <c r="P26" s="170"/>
+      <c r="Q26" s="170"/>
+      <c r="R26" s="170"/>
     </row>
     <row r="28" spans="1:195" ht="18">
-      <c r="B28" s="157"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="157"/>
-      <c r="L28" s="157"/>
-      <c r="M28" s="157"/>
-      <c r="N28" s="157"/>
-      <c r="O28" s="157"/>
-      <c r="P28" s="157"/>
-      <c r="Q28" s="157"/>
-      <c r="R28" s="157"/>
-      <c r="S28" s="155"/>
-      <c r="T28" s="155"/>
-      <c r="U28" s="155"/>
-      <c r="V28" s="155"/>
-      <c r="W28" s="155"/>
-      <c r="X28" s="155"/>
-      <c r="Y28" s="155"/>
-      <c r="Z28" s="155"/>
-      <c r="AA28" s="155"/>
-      <c r="AB28" s="155"/>
-      <c r="AC28" s="155"/>
-      <c r="AD28" s="155"/>
-      <c r="AE28" s="155"/>
-      <c r="AF28" s="155"/>
-      <c r="AG28" s="155"/>
-      <c r="AH28" s="155"/>
-      <c r="AI28" s="155"/>
-      <c r="AJ28" s="155"/>
-      <c r="AK28" s="155"/>
-      <c r="AL28" s="155"/>
-      <c r="AM28" s="155"/>
-      <c r="AN28" s="155"/>
-      <c r="AO28" s="155"/>
-      <c r="AP28" s="155"/>
-      <c r="AQ28" s="155"/>
-      <c r="AR28" s="155"/>
-      <c r="AS28" s="155"/>
-      <c r="AT28" s="155"/>
-      <c r="AU28" s="155"/>
-      <c r="AV28" s="155"/>
-      <c r="AW28" s="155"/>
-      <c r="AX28" s="155"/>
-      <c r="AY28" s="155"/>
-      <c r="AZ28" s="155"/>
-      <c r="BA28" s="155"/>
-      <c r="BB28" s="155"/>
-      <c r="BC28" s="155"/>
-      <c r="BD28" s="155"/>
-      <c r="BE28" s="155"/>
-      <c r="BF28" s="155"/>
-      <c r="BG28" s="155"/>
-      <c r="BH28" s="155"/>
-      <c r="BI28" s="155"/>
-      <c r="BJ28" s="155"/>
-      <c r="BK28" s="155"/>
-      <c r="BL28" s="155"/>
-      <c r="BM28" s="155"/>
-      <c r="BN28" s="155"/>
-      <c r="BO28" s="155"/>
-      <c r="BP28" s="155"/>
-      <c r="BQ28" s="155"/>
-      <c r="BR28" s="155"/>
-      <c r="BS28" s="155"/>
-      <c r="BT28" s="155"/>
-      <c r="BU28" s="155"/>
-      <c r="BV28" s="155"/>
-      <c r="BW28" s="155"/>
-      <c r="BX28" s="155"/>
-      <c r="BY28" s="155"/>
-      <c r="BZ28" s="155"/>
-      <c r="CA28" s="155"/>
-      <c r="CB28" s="155"/>
-      <c r="CC28" s="155"/>
-      <c r="CD28" s="155"/>
-      <c r="CE28" s="155"/>
-      <c r="CF28" s="155"/>
-      <c r="CG28" s="155"/>
-      <c r="CH28" s="155"/>
-      <c r="CI28" s="155"/>
-      <c r="CJ28" s="155"/>
-      <c r="CK28" s="155"/>
-      <c r="CL28" s="155"/>
-      <c r="CM28" s="155"/>
-      <c r="CN28" s="155"/>
-      <c r="CO28" s="155"/>
-      <c r="CP28" s="155"/>
-      <c r="CQ28" s="155"/>
-      <c r="CR28" s="155"/>
-      <c r="CS28" s="155"/>
-      <c r="CT28" s="155"/>
-      <c r="CU28" s="155"/>
-      <c r="CV28" s="155"/>
-      <c r="CW28" s="155"/>
-      <c r="CX28" s="155"/>
-      <c r="CY28" s="155"/>
-      <c r="CZ28" s="155"/>
-      <c r="DA28" s="155"/>
-      <c r="DB28" s="155"/>
-      <c r="DC28" s="155"/>
-      <c r="DD28" s="155"/>
-      <c r="DE28" s="155"/>
-      <c r="DF28" s="155"/>
-      <c r="DG28" s="155"/>
-      <c r="DH28" s="155"/>
-      <c r="DI28" s="155"/>
-      <c r="DJ28" s="155"/>
-      <c r="DK28" s="155"/>
-      <c r="DL28" s="155"/>
-      <c r="DM28" s="155"/>
-      <c r="DN28" s="155"/>
-      <c r="DO28" s="155"/>
-      <c r="DP28" s="155"/>
-      <c r="DQ28" s="155"/>
-      <c r="DR28" s="155"/>
-      <c r="DS28" s="155"/>
-      <c r="DT28" s="155"/>
-      <c r="DU28" s="155"/>
-      <c r="DV28" s="155"/>
-      <c r="DW28" s="155"/>
-      <c r="DX28" s="155"/>
-      <c r="DY28" s="155"/>
-      <c r="DZ28" s="155"/>
-      <c r="EA28" s="155"/>
-      <c r="EB28" s="155"/>
-      <c r="EC28" s="155"/>
-      <c r="ED28" s="155"/>
-      <c r="EE28" s="155"/>
-      <c r="EF28" s="155"/>
-      <c r="EG28" s="155"/>
-      <c r="EH28" s="155"/>
-      <c r="EI28" s="155"/>
-      <c r="EJ28" s="155"/>
-      <c r="EK28" s="155"/>
-      <c r="EL28" s="155"/>
-      <c r="EM28" s="155"/>
-      <c r="EN28" s="155"/>
-      <c r="EO28" s="155"/>
-      <c r="EP28" s="155"/>
-      <c r="EQ28" s="155"/>
-      <c r="ER28" s="155"/>
-      <c r="ES28" s="155"/>
-      <c r="ET28" s="155"/>
-      <c r="EU28" s="155"/>
-      <c r="EV28" s="155"/>
-      <c r="EW28" s="155"/>
-      <c r="EX28" s="155"/>
-      <c r="EY28" s="155"/>
-      <c r="EZ28" s="155"/>
-      <c r="FA28" s="155"/>
-      <c r="FB28" s="155"/>
-      <c r="FC28" s="155"/>
-      <c r="FD28" s="155"/>
-      <c r="FE28" s="155"/>
-      <c r="FF28" s="155"/>
-      <c r="FG28" s="155"/>
-      <c r="FH28" s="155"/>
-      <c r="FI28" s="155"/>
-      <c r="FJ28" s="155"/>
-      <c r="FK28" s="155"/>
-      <c r="FL28" s="155"/>
-      <c r="FM28" s="155"/>
-      <c r="FN28" s="155"/>
-      <c r="FO28" s="155"/>
-      <c r="FP28" s="155"/>
-      <c r="FQ28" s="155"/>
-      <c r="FR28" s="155"/>
-      <c r="FS28" s="155"/>
-      <c r="FT28" s="155"/>
-      <c r="FU28" s="155"/>
-      <c r="FV28" s="155"/>
-      <c r="FW28" s="155"/>
-      <c r="FX28" s="155"/>
-      <c r="FY28" s="155"/>
-      <c r="FZ28" s="155"/>
-      <c r="GA28" s="155"/>
-      <c r="GB28" s="155"/>
-      <c r="GC28" s="155"/>
-      <c r="GD28" s="155"/>
-      <c r="GE28" s="155"/>
-      <c r="GF28" s="155"/>
-      <c r="GG28" s="155"/>
-      <c r="GH28" s="155"/>
-      <c r="GI28" s="155"/>
-      <c r="GJ28" s="155"/>
-      <c r="GK28" s="155"/>
-      <c r="GL28" s="155"/>
+      <c r="B28" s="172"/>
+      <c r="C28" s="172"/>
+      <c r="D28" s="172"/>
+      <c r="E28" s="172"/>
+      <c r="F28" s="172"/>
+      <c r="G28" s="172"/>
+      <c r="H28" s="172"/>
+      <c r="I28" s="172"/>
+      <c r="J28" s="172"/>
+      <c r="K28" s="172"/>
+      <c r="L28" s="172"/>
+      <c r="M28" s="172"/>
+      <c r="N28" s="172"/>
+      <c r="O28" s="172"/>
+      <c r="P28" s="172"/>
+      <c r="Q28" s="172"/>
+      <c r="R28" s="172"/>
+      <c r="S28" s="171"/>
+      <c r="T28" s="171"/>
+      <c r="U28" s="171"/>
+      <c r="V28" s="171"/>
+      <c r="W28" s="171"/>
+      <c r="X28" s="171"/>
+      <c r="Y28" s="171"/>
+      <c r="Z28" s="171"/>
+      <c r="AA28" s="171"/>
+      <c r="AB28" s="171"/>
+      <c r="AC28" s="171"/>
+      <c r="AD28" s="171"/>
+      <c r="AE28" s="171"/>
+      <c r="AF28" s="171"/>
+      <c r="AG28" s="171"/>
+      <c r="AH28" s="171"/>
+      <c r="AI28" s="171"/>
+      <c r="AJ28" s="171"/>
+      <c r="AK28" s="171"/>
+      <c r="AL28" s="171"/>
+      <c r="AM28" s="171"/>
+      <c r="AN28" s="171"/>
+      <c r="AO28" s="171"/>
+      <c r="AP28" s="171"/>
+      <c r="AQ28" s="171"/>
+      <c r="AR28" s="171"/>
+      <c r="AS28" s="171"/>
+      <c r="AT28" s="171"/>
+      <c r="AU28" s="171"/>
+      <c r="AV28" s="171"/>
+      <c r="AW28" s="171"/>
+      <c r="AX28" s="171"/>
+      <c r="AY28" s="171"/>
+      <c r="AZ28" s="171"/>
+      <c r="BA28" s="171"/>
+      <c r="BB28" s="171"/>
+      <c r="BC28" s="171"/>
+      <c r="BD28" s="171"/>
+      <c r="BE28" s="171"/>
+      <c r="BF28" s="171"/>
+      <c r="BG28" s="171"/>
+      <c r="BH28" s="171"/>
+      <c r="BI28" s="171"/>
+      <c r="BJ28" s="171"/>
+      <c r="BK28" s="171"/>
+      <c r="BL28" s="171"/>
+      <c r="BM28" s="171"/>
+      <c r="BN28" s="171"/>
+      <c r="BO28" s="171"/>
+      <c r="BP28" s="171"/>
+      <c r="BQ28" s="171"/>
+      <c r="BR28" s="171"/>
+      <c r="BS28" s="171"/>
+      <c r="BT28" s="171"/>
+      <c r="BU28" s="171"/>
+      <c r="BV28" s="171"/>
+      <c r="BW28" s="171"/>
+      <c r="BX28" s="171"/>
+      <c r="BY28" s="171"/>
+      <c r="BZ28" s="171"/>
+      <c r="CA28" s="171"/>
+      <c r="CB28" s="171"/>
+      <c r="CC28" s="171"/>
+      <c r="CD28" s="171"/>
+      <c r="CE28" s="171"/>
+      <c r="CF28" s="171"/>
+      <c r="CG28" s="171"/>
+      <c r="CH28" s="171"/>
+      <c r="CI28" s="171"/>
+      <c r="CJ28" s="171"/>
+      <c r="CK28" s="171"/>
+      <c r="CL28" s="171"/>
+      <c r="CM28" s="171"/>
+      <c r="CN28" s="171"/>
+      <c r="CO28" s="171"/>
+      <c r="CP28" s="171"/>
+      <c r="CQ28" s="171"/>
+      <c r="CR28" s="171"/>
+      <c r="CS28" s="171"/>
+      <c r="CT28" s="171"/>
+      <c r="CU28" s="171"/>
+      <c r="CV28" s="171"/>
+      <c r="CW28" s="171"/>
+      <c r="CX28" s="171"/>
+      <c r="CY28" s="171"/>
+      <c r="CZ28" s="171"/>
+      <c r="DA28" s="171"/>
+      <c r="DB28" s="171"/>
+      <c r="DC28" s="171"/>
+      <c r="DD28" s="171"/>
+      <c r="DE28" s="171"/>
+      <c r="DF28" s="171"/>
+      <c r="DG28" s="171"/>
+      <c r="DH28" s="171"/>
+      <c r="DI28" s="171"/>
+      <c r="DJ28" s="171"/>
+      <c r="DK28" s="171"/>
+      <c r="DL28" s="171"/>
+      <c r="DM28" s="171"/>
+      <c r="DN28" s="171"/>
+      <c r="DO28" s="171"/>
+      <c r="DP28" s="171"/>
+      <c r="DQ28" s="171"/>
+      <c r="DR28" s="171"/>
+      <c r="DS28" s="171"/>
+      <c r="DT28" s="171"/>
+      <c r="DU28" s="171"/>
+      <c r="DV28" s="171"/>
+      <c r="DW28" s="171"/>
+      <c r="DX28" s="171"/>
+      <c r="DY28" s="171"/>
+      <c r="DZ28" s="171"/>
+      <c r="EA28" s="171"/>
+      <c r="EB28" s="171"/>
+      <c r="EC28" s="171"/>
+      <c r="ED28" s="171"/>
+      <c r="EE28" s="171"/>
+      <c r="EF28" s="171"/>
+      <c r="EG28" s="171"/>
+      <c r="EH28" s="171"/>
+      <c r="EI28" s="171"/>
+      <c r="EJ28" s="171"/>
+      <c r="EK28" s="171"/>
+      <c r="EL28" s="171"/>
+      <c r="EM28" s="171"/>
+      <c r="EN28" s="171"/>
+      <c r="EO28" s="171"/>
+      <c r="EP28" s="171"/>
+      <c r="EQ28" s="171"/>
+      <c r="ER28" s="171"/>
+      <c r="ES28" s="171"/>
+      <c r="ET28" s="171"/>
+      <c r="EU28" s="171"/>
+      <c r="EV28" s="171"/>
+      <c r="EW28" s="171"/>
+      <c r="EX28" s="171"/>
+      <c r="EY28" s="171"/>
+      <c r="EZ28" s="171"/>
+      <c r="FA28" s="171"/>
+      <c r="FB28" s="171"/>
+      <c r="FC28" s="171"/>
+      <c r="FD28" s="171"/>
+      <c r="FE28" s="171"/>
+      <c r="FF28" s="171"/>
+      <c r="FG28" s="171"/>
+      <c r="FH28" s="171"/>
+      <c r="FI28" s="171"/>
+      <c r="FJ28" s="171"/>
+      <c r="FK28" s="171"/>
+      <c r="FL28" s="171"/>
+      <c r="FM28" s="171"/>
+      <c r="FN28" s="171"/>
+      <c r="FO28" s="171"/>
+      <c r="FP28" s="171"/>
+      <c r="FQ28" s="171"/>
+      <c r="FR28" s="171"/>
+      <c r="FS28" s="171"/>
+      <c r="FT28" s="171"/>
+      <c r="FU28" s="171"/>
+      <c r="FV28" s="171"/>
+      <c r="FW28" s="171"/>
+      <c r="FX28" s="171"/>
+      <c r="FY28" s="171"/>
+      <c r="FZ28" s="171"/>
+      <c r="GA28" s="171"/>
+      <c r="GB28" s="171"/>
+      <c r="GC28" s="171"/>
+      <c r="GD28" s="171"/>
+      <c r="GE28" s="171"/>
+      <c r="GF28" s="171"/>
+      <c r="GG28" s="171"/>
+      <c r="GH28" s="171"/>
+      <c r="GI28" s="171"/>
+      <c r="GJ28" s="171"/>
+      <c r="GK28" s="171"/>
+      <c r="GL28" s="171"/>
       <c r="GM28" s="101"/>
     </row>
     <row r="29" spans="1:195" ht="18">
-      <c r="B29" s="156"/>
-      <c r="C29" s="156"/>
-      <c r="D29" s="156"/>
-      <c r="E29" s="156"/>
-      <c r="F29" s="156"/>
-      <c r="G29" s="156"/>
-      <c r="H29" s="156"/>
-      <c r="I29" s="156"/>
-      <c r="J29" s="156"/>
-      <c r="K29" s="156"/>
-      <c r="L29" s="156"/>
-      <c r="M29" s="156"/>
-      <c r="N29" s="156"/>
-      <c r="O29" s="156"/>
-      <c r="P29" s="156"/>
-      <c r="Q29" s="156"/>
-      <c r="R29" s="156"/>
+      <c r="B29" s="170"/>
+      <c r="C29" s="170"/>
+      <c r="D29" s="170"/>
+      <c r="E29" s="170"/>
+      <c r="F29" s="170"/>
+      <c r="G29" s="170"/>
+      <c r="H29" s="170"/>
+      <c r="I29" s="170"/>
+      <c r="J29" s="170"/>
+      <c r="K29" s="170"/>
+      <c r="L29" s="170"/>
+      <c r="M29" s="170"/>
+      <c r="N29" s="170"/>
+      <c r="O29" s="170"/>
+      <c r="P29" s="170"/>
+      <c r="Q29" s="170"/>
+      <c r="R29" s="170"/>
     </row>
     <row r="30" spans="1:195" ht="13.5" customHeight="1">
-      <c r="A30" s="154"/>
-      <c r="B30" s="154"/>
-      <c r="C30" s="154"/>
-      <c r="D30" s="154"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="154"/>
-      <c r="G30" s="154"/>
-      <c r="H30" s="154"/>
-      <c r="I30" s="154"/>
-      <c r="J30" s="154"/>
+      <c r="A30" s="173"/>
+      <c r="B30" s="173"/>
+      <c r="C30" s="173"/>
+      <c r="D30" s="173"/>
+      <c r="E30" s="173"/>
+      <c r="F30" s="173"/>
+      <c r="G30" s="173"/>
+      <c r="H30" s="173"/>
+      <c r="I30" s="173"/>
+      <c r="J30" s="173"/>
       <c r="K30" s="102"/>
       <c r="L30" s="102"/>
       <c r="M30" s="102"/>
@@ -5265,16 +5387,16 @@
       <c r="R30" s="102"/>
     </row>
     <row r="31" spans="1:195" ht="13.5" customHeight="1">
-      <c r="A31" s="154"/>
-      <c r="B31" s="154"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="154"/>
-      <c r="E31" s="154"/>
-      <c r="F31" s="154"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="154"/>
+      <c r="A31" s="173"/>
+      <c r="B31" s="173"/>
+      <c r="C31" s="173"/>
+      <c r="D31" s="173"/>
+      <c r="E31" s="173"/>
+      <c r="F31" s="173"/>
+      <c r="G31" s="173"/>
+      <c r="H31" s="173"/>
+      <c r="I31" s="173"/>
+      <c r="J31" s="173"/>
       <c r="K31" s="102"/>
       <c r="L31" s="102"/>
       <c r="M31" s="102"/>
@@ -5286,6 +5408,28 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="DF28:DV28"/>
+    <mergeCell ref="DW28:EM28"/>
+    <mergeCell ref="EN28:FD28"/>
+    <mergeCell ref="B26:R26"/>
+    <mergeCell ref="FE28:FU28"/>
+    <mergeCell ref="FV28:GL28"/>
+    <mergeCell ref="B29:R29"/>
+    <mergeCell ref="S28:X28"/>
+    <mergeCell ref="Y28:AO28"/>
+    <mergeCell ref="AP28:BF28"/>
+    <mergeCell ref="BG28:BW28"/>
+    <mergeCell ref="BX28:CN28"/>
+    <mergeCell ref="CO28:DE28"/>
+    <mergeCell ref="B28:R28"/>
+    <mergeCell ref="B18:R18"/>
+    <mergeCell ref="B20:R20"/>
+    <mergeCell ref="B21:R21"/>
+    <mergeCell ref="B22:R22"/>
+    <mergeCell ref="B23:R23"/>
+    <mergeCell ref="B19:R19"/>
     <mergeCell ref="B14:R14"/>
     <mergeCell ref="B15:R15"/>
     <mergeCell ref="A16:J16"/>
@@ -5299,28 +5443,6 @@
     <mergeCell ref="C1:F3"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B18:R18"/>
-    <mergeCell ref="B20:R20"/>
-    <mergeCell ref="B21:R21"/>
-    <mergeCell ref="B22:R22"/>
-    <mergeCell ref="B23:R23"/>
-    <mergeCell ref="B19:R19"/>
-    <mergeCell ref="B26:R26"/>
-    <mergeCell ref="FE28:FU28"/>
-    <mergeCell ref="FV28:GL28"/>
-    <mergeCell ref="B29:R29"/>
-    <mergeCell ref="S28:X28"/>
-    <mergeCell ref="Y28:AO28"/>
-    <mergeCell ref="AP28:BF28"/>
-    <mergeCell ref="BG28:BW28"/>
-    <mergeCell ref="BX28:CN28"/>
-    <mergeCell ref="CO28:DE28"/>
-    <mergeCell ref="B28:R28"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="DF28:DV28"/>
-    <mergeCell ref="DW28:EM28"/>
-    <mergeCell ref="EN28:FD28"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.39370078740157499" bottom="0" header="0" footer="0"/>
@@ -5332,9 +5454,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G62"/>
+  <dimension ref="B1:J62"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A8" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -5347,14 +5469,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14.25">
-      <c r="B1" s="240" t="s">
+      <c r="B1" s="232" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
+      <c r="C1" s="232"/>
+      <c r="D1" s="232"/>
+      <c r="E1" s="232"/>
+      <c r="F1" s="232"/>
+      <c r="G1" s="232"/>
     </row>
     <row r="2" spans="2:7" s="17" customFormat="1">
       <c r="B2" s="16"/>
@@ -5450,7 +5572,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:10">
       <c r="E17" s="6" t="s">
         <v>16</v>
       </c>
@@ -5461,7 +5583,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:10">
       <c r="E18" s="8" t="s">
         <v>18</v>
       </c>
@@ -5472,7 +5594,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:10">
       <c r="E19" s="9" t="s">
         <v>20</v>
       </c>
@@ -5483,7 +5605,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:10">
       <c r="E20" s="10" t="s">
         <v>22</v>
       </c>
@@ -5494,7 +5616,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:10">
       <c r="E21" s="11" t="s">
         <v>24</v>
       </c>
@@ -5505,7 +5627,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:10">
       <c r="E22" s="12" t="s">
         <v>26</v>
       </c>
@@ -5516,7 +5638,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:10">
       <c r="E23" s="13" t="s">
         <v>28</v>
       </c>
@@ -5527,7 +5649,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:10">
       <c r="E24" s="14" t="s">
         <v>30</v>
       </c>
@@ -5538,7 +5660,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="2:7" s="18" customFormat="1" ht="15.75" customHeight="1">
+    <row r="26" spans="2:10" s="18" customFormat="1" ht="15.75" customHeight="1">
       <c r="D26" s="18" t="s">
         <v>65</v>
       </c>
@@ -5546,31 +5668,34 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="200.25" customHeight="1">
-      <c r="E27" s="241" t="s">
+    <row r="27" spans="2:10" ht="200.25" customHeight="1">
+      <c r="E27" s="233" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="242"/>
-      <c r="G27" s="243"/>
-    </row>
-    <row r="29" spans="2:7">
+      <c r="F27" s="234"/>
+      <c r="G27" s="235"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="J28" s="236"/>
+    </row>
+    <row r="29" spans="2:10">
       <c r="B29" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:10">
       <c r="B30" s="19"/>
       <c r="C30" s="20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="2:7">
+    <row r="31" spans="2:10">
       <c r="B31" s="19"/>
       <c r="C31" s="20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:7">
+    <row r="32" spans="2:10">
       <c r="D32" s="1" t="s">
         <v>62</v>
       </c>
@@ -5849,75 +5974,75 @@
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B12" s="143" t="s">
+      <c r="B12" s="142" t="s">
+        <v>299</v>
+      </c>
+      <c r="C12" s="90" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B13" s="142" t="s">
+        <v>301</v>
+      </c>
+      <c r="C13" s="90" t="s">
         <v>302</v>
       </c>
-      <c r="C12" s="90" t="s">
+    </row>
+    <row r="14" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B14" s="142" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B13" s="143" t="s">
+      <c r="C14" s="90" t="s">
         <v>304</v>
       </c>
-      <c r="C13" s="90" t="s">
+    </row>
+    <row r="15" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B15" s="142" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B14" s="143" t="s">
+      <c r="C15" s="90" t="s">
         <v>306</v>
       </c>
-      <c r="C14" s="90" t="s">
+    </row>
+    <row r="16" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B16" s="142" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B15" s="143" t="s">
+      <c r="C16" s="90" t="s">
         <v>308</v>
       </c>
-      <c r="C15" s="90" t="s">
+    </row>
+    <row r="17" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B17" s="142" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B16" s="143" t="s">
+      <c r="C17" s="90" t="s">
         <v>310</v>
       </c>
-      <c r="C16" s="90" t="s">
+    </row>
+    <row r="18" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B18" s="142" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B17" s="143" t="s">
+      <c r="C18" s="90" t="s">
         <v>312</v>
       </c>
-      <c r="C17" s="90" t="s">
+    </row>
+    <row r="19" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B19" s="142" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B18" s="143" t="s">
+      <c r="C19" s="90" t="s">
         <v>314</v>
       </c>
-      <c r="C18" s="90" t="s">
+    </row>
+    <row r="20" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B20" s="142" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B19" s="143" t="s">
+      <c r="C20" s="90" t="s">
         <v>316</v>
-      </c>
-      <c r="C19" s="90" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B20" s="143" t="s">
-        <v>318</v>
-      </c>
-      <c r="C20" s="90" t="s">
-        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -5930,8 +6055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:J10"/>
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -5947,10 +6072,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="183"/>
+      <c r="B1" s="174"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -5977,8 +6102,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="183"/>
-      <c r="B2" s="183"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="174"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -6017,14 +6142,14 @@
       <c r="D4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="184" t="s">
+      <c r="E4" s="175" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="184"/>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="184"/>
+      <c r="F4" s="175"/>
+      <c r="G4" s="175"/>
+      <c r="H4" s="175"/>
+      <c r="I4" s="175"/>
+      <c r="J4" s="175"/>
     </row>
     <row r="5" spans="1:10" ht="24.75" customHeight="1">
       <c r="A5" s="36">
@@ -6055,20 +6180,20 @@
       <c r="B6" s="37">
         <v>2</v>
       </c>
-      <c r="C6" s="144" t="s">
+      <c r="C6" s="143" t="s">
         <v>208</v>
       </c>
-      <c r="D6" s="144">
+      <c r="D6" s="143">
         <v>42860</v>
       </c>
-      <c r="E6" s="185" t="s">
-        <v>323</v>
-      </c>
-      <c r="F6" s="186"/>
-      <c r="G6" s="186"/>
-      <c r="H6" s="186"/>
-      <c r="I6" s="186"/>
-      <c r="J6" s="187"/>
+      <c r="E6" s="177" t="s">
+        <v>317</v>
+      </c>
+      <c r="F6" s="178"/>
+      <c r="G6" s="178"/>
+      <c r="H6" s="178"/>
+      <c r="I6" s="178"/>
+      <c r="J6" s="179"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1">
       <c r="A7" s="72">
@@ -6077,14 +6202,20 @@
       <c r="B7" s="37">
         <v>3</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="177"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="178"/>
-      <c r="H7" s="178"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="179"/>
+      <c r="C7" s="237" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" s="238" t="s">
+        <v>319</v>
+      </c>
+      <c r="E7" s="239" t="s">
+        <v>320</v>
+      </c>
+      <c r="F7" s="240"/>
+      <c r="G7" s="240"/>
+      <c r="H7" s="240"/>
+      <c r="I7" s="240"/>
+      <c r="J7" s="241"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
       <c r="A8" s="73">
@@ -6095,12 +6226,12 @@
       </c>
       <c r="C8" s="65"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="182"/>
+      <c r="E8" s="183"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="184"/>
+      <c r="H8" s="184"/>
+      <c r="I8" s="184"/>
+      <c r="J8" s="185"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
       <c r="A9" s="74">
@@ -6111,12 +6242,12 @@
       </c>
       <c r="C9" s="65"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="177"/>
-      <c r="F9" s="178"/>
-      <c r="G9" s="178"/>
-      <c r="H9" s="178"/>
-      <c r="I9" s="178"/>
-      <c r="J9" s="179"/>
+      <c r="E9" s="180"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="181"/>
+      <c r="J9" s="182"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1">
       <c r="A10" s="75">
@@ -6127,12 +6258,12 @@
       </c>
       <c r="C10" s="65"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="177"/>
-      <c r="F10" s="178"/>
-      <c r="G10" s="178"/>
-      <c r="H10" s="178"/>
-      <c r="I10" s="178"/>
-      <c r="J10" s="179"/>
+      <c r="E10" s="180"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="182"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
       <c r="A11" s="76">
@@ -6143,12 +6274,12 @@
       </c>
       <c r="C11" s="65"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="177"/>
-      <c r="F11" s="178"/>
-      <c r="G11" s="178"/>
-      <c r="H11" s="178"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="179"/>
+      <c r="E11" s="180"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="182"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1">
       <c r="A12" s="77">
@@ -6159,12 +6290,12 @@
       </c>
       <c r="C12" s="65"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="177"/>
-      <c r="F12" s="178"/>
-      <c r="G12" s="178"/>
-      <c r="H12" s="178"/>
-      <c r="I12" s="178"/>
-      <c r="J12" s="179"/>
+      <c r="E12" s="180"/>
+      <c r="F12" s="181"/>
+      <c r="G12" s="181"/>
+      <c r="H12" s="181"/>
+      <c r="I12" s="181"/>
+      <c r="J12" s="182"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
       <c r="A13" s="78">
@@ -6175,12 +6306,12 @@
       </c>
       <c r="C13" s="65"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="177"/>
-      <c r="F13" s="178"/>
-      <c r="G13" s="178"/>
-      <c r="H13" s="178"/>
-      <c r="I13" s="178"/>
-      <c r="J13" s="179"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="181"/>
+      <c r="G13" s="181"/>
+      <c r="H13" s="181"/>
+      <c r="I13" s="181"/>
+      <c r="J13" s="182"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
       <c r="A14" s="79">
@@ -6191,12 +6322,12 @@
       </c>
       <c r="C14" s="65"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="177"/>
-      <c r="F14" s="178"/>
-      <c r="G14" s="178"/>
-      <c r="H14" s="178"/>
-      <c r="I14" s="178"/>
-      <c r="J14" s="179"/>
+      <c r="E14" s="180"/>
+      <c r="F14" s="181"/>
+      <c r="G14" s="181"/>
+      <c r="H14" s="181"/>
+      <c r="I14" s="181"/>
+      <c r="J14" s="182"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
       <c r="A15" s="36">
@@ -6520,17 +6651,11 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
     <mergeCell ref="E31:J31"/>
     <mergeCell ref="E32:J32"/>
     <mergeCell ref="E33:J33"/>
@@ -6547,11 +6672,17 @@
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="E13:J13"/>
     <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E22:J22"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -6576,7 +6707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="I12" sqref="I12:J44"/>
     </sheetView>
   </sheetViews>
@@ -6596,10 +6727,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="183"/>
+      <c r="B1" s="174"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -6630,8 +6761,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="183"/>
-      <c r="B2" s="183"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="174"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -6662,20 +6793,20 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1">
-      <c r="A4" s="188" t="s">
+      <c r="A4" s="186" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="190"/>
-      <c r="D4" s="190"/>
-      <c r="E4" s="190"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="190"/>
-      <c r="H4" s="189"/>
-      <c r="I4" s="188" t="s">
+      <c r="B4" s="188"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="186" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="189"/>
+      <c r="J4" s="187"/>
     </row>
     <row r="5" spans="1:10" ht="12" customHeight="1">
       <c r="A5"/>
@@ -6686,10 +6817,10 @@
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
       <c r="H5" s="40"/>
-      <c r="I5" s="195" t="s">
+      <c r="I5" s="193" t="s">
         <v>247</v>
       </c>
-      <c r="J5" s="196"/>
+      <c r="J5" s="194"/>
     </row>
     <row r="6" spans="1:10" ht="12" customHeight="1">
       <c r="A6" s="38"/>
@@ -6700,8 +6831,8 @@
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
       <c r="H6" s="41"/>
-      <c r="I6" s="197"/>
-      <c r="J6" s="198"/>
+      <c r="I6" s="195"/>
+      <c r="J6" s="196"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1">
       <c r="A7" s="38"/>
@@ -6712,8 +6843,8 @@
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
       <c r="H7" s="41"/>
-      <c r="I7" s="197"/>
-      <c r="J7" s="198"/>
+      <c r="I7" s="195"/>
+      <c r="J7" s="196"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
       <c r="A8" s="38"/>
@@ -6724,8 +6855,8 @@
       <c r="F8" s="39"/>
       <c r="G8" s="39"/>
       <c r="H8" s="41"/>
-      <c r="I8" s="197"/>
-      <c r="J8" s="198"/>
+      <c r="I8" s="195"/>
+      <c r="J8" s="196"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
       <c r="A9" s="38"/>
@@ -6736,8 +6867,8 @@
       <c r="F9" s="39"/>
       <c r="G9" s="39"/>
       <c r="H9" s="41"/>
-      <c r="I9" s="197"/>
-      <c r="J9" s="198"/>
+      <c r="I9" s="195"/>
+      <c r="J9" s="196"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1">
       <c r="A10" s="38"/>
@@ -6748,8 +6879,8 @@
       <c r="F10" s="39"/>
       <c r="G10" s="39"/>
       <c r="H10" s="41"/>
-      <c r="I10" s="199"/>
-      <c r="J10" s="200"/>
+      <c r="I10" s="197"/>
+      <c r="J10" s="198"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
       <c r="A11" s="38"/>
@@ -6760,10 +6891,10 @@
       <c r="F11" s="39"/>
       <c r="G11" s="39"/>
       <c r="H11" s="42"/>
-      <c r="I11" s="188" t="s">
+      <c r="I11" s="186" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="189"/>
+      <c r="J11" s="187"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1">
       <c r="A12" s="38"/>
@@ -6774,10 +6905,10 @@
       <c r="F12" s="39"/>
       <c r="G12" s="39"/>
       <c r="H12" s="41"/>
-      <c r="I12" s="191" t="s">
+      <c r="I12" s="189" t="s">
         <v>248</v>
       </c>
-      <c r="J12" s="192"/>
+      <c r="J12" s="190"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
       <c r="A13" s="38"/>
@@ -6788,8 +6919,8 @@
       <c r="F13" s="39"/>
       <c r="G13" s="39"/>
       <c r="H13" s="41"/>
-      <c r="I13" s="193"/>
-      <c r="J13" s="194"/>
+      <c r="I13" s="191"/>
+      <c r="J13" s="192"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
       <c r="A14" s="38"/>
@@ -6800,8 +6931,8 @@
       <c r="F14" s="39"/>
       <c r="G14" s="39"/>
       <c r="H14" s="41"/>
-      <c r="I14" s="193"/>
-      <c r="J14" s="194"/>
+      <c r="I14" s="191"/>
+      <c r="J14" s="192"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
       <c r="A15" s="38"/>
@@ -6812,8 +6943,8 @@
       <c r="F15" s="39"/>
       <c r="G15" s="39"/>
       <c r="H15" s="41"/>
-      <c r="I15" s="193"/>
-      <c r="J15" s="194"/>
+      <c r="I15" s="191"/>
+      <c r="J15" s="192"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
       <c r="A16" s="38"/>
@@ -6824,8 +6955,8 @@
       <c r="F16" s="39"/>
       <c r="G16" s="39"/>
       <c r="H16" s="41"/>
-      <c r="I16" s="193"/>
-      <c r="J16" s="194"/>
+      <c r="I16" s="191"/>
+      <c r="J16" s="192"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1">
       <c r="A17" s="38"/>
@@ -6836,8 +6967,8 @@
       <c r="F17" s="39"/>
       <c r="G17" s="39"/>
       <c r="H17" s="41"/>
-      <c r="I17" s="193"/>
-      <c r="J17" s="194"/>
+      <c r="I17" s="191"/>
+      <c r="J17" s="192"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1">
       <c r="A18" s="38"/>
@@ -6848,8 +6979,8 @@
       <c r="F18" s="39"/>
       <c r="G18" s="39"/>
       <c r="H18" s="41"/>
-      <c r="I18" s="193"/>
-      <c r="J18" s="194"/>
+      <c r="I18" s="191"/>
+      <c r="J18" s="192"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1">
       <c r="A19" s="38"/>
@@ -6860,8 +6991,8 @@
       <c r="F19" s="39"/>
       <c r="G19" s="39"/>
       <c r="H19" s="41"/>
-      <c r="I19" s="193"/>
-      <c r="J19" s="194"/>
+      <c r="I19" s="191"/>
+      <c r="J19" s="192"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1">
       <c r="A20" s="38"/>
@@ -6872,8 +7003,8 @@
       <c r="F20" s="39"/>
       <c r="G20" s="39"/>
       <c r="H20" s="41"/>
-      <c r="I20" s="193"/>
-      <c r="J20" s="194"/>
+      <c r="I20" s="191"/>
+      <c r="J20" s="192"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
       <c r="A21" s="38"/>
@@ -6884,8 +7015,8 @@
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
       <c r="H21" s="41"/>
-      <c r="I21" s="193"/>
-      <c r="J21" s="194"/>
+      <c r="I21" s="191"/>
+      <c r="J21" s="192"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="A22" s="38"/>
@@ -6896,8 +7027,8 @@
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
       <c r="H22" s="41"/>
-      <c r="I22" s="193"/>
-      <c r="J22" s="194"/>
+      <c r="I22" s="191"/>
+      <c r="J22" s="192"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1">
       <c r="A23" s="38"/>
@@ -6908,8 +7039,8 @@
       <c r="F23" s="39"/>
       <c r="G23" s="39"/>
       <c r="H23" s="41"/>
-      <c r="I23" s="193"/>
-      <c r="J23" s="194"/>
+      <c r="I23" s="191"/>
+      <c r="J23" s="192"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1">
       <c r="A24" s="38"/>
@@ -6920,8 +7051,8 @@
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
       <c r="H24" s="41"/>
-      <c r="I24" s="193"/>
-      <c r="J24" s="194"/>
+      <c r="I24" s="191"/>
+      <c r="J24" s="192"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1">
       <c r="A25" s="38"/>
@@ -6932,8 +7063,8 @@
       <c r="F25" s="39"/>
       <c r="G25" s="39"/>
       <c r="H25" s="41"/>
-      <c r="I25" s="193"/>
-      <c r="J25" s="194"/>
+      <c r="I25" s="191"/>
+      <c r="J25" s="192"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="38"/>
@@ -6944,8 +7075,8 @@
       <c r="F26" s="39"/>
       <c r="G26" s="39"/>
       <c r="H26" s="41"/>
-      <c r="I26" s="193"/>
-      <c r="J26" s="194"/>
+      <c r="I26" s="191"/>
+      <c r="J26" s="192"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1">
       <c r="A27" s="38"/>
@@ -6956,8 +7087,8 @@
       <c r="F27" s="39"/>
       <c r="G27" s="39"/>
       <c r="H27" s="41"/>
-      <c r="I27" s="193"/>
-      <c r="J27" s="194"/>
+      <c r="I27" s="191"/>
+      <c r="J27" s="192"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1">
       <c r="A28" s="38"/>
@@ -6968,8 +7099,8 @@
       <c r="F28" s="39"/>
       <c r="G28" s="39"/>
       <c r="H28" s="41"/>
-      <c r="I28" s="193"/>
-      <c r="J28" s="194"/>
+      <c r="I28" s="191"/>
+      <c r="J28" s="192"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1">
       <c r="A29" s="38"/>
@@ -6980,8 +7111,8 @@
       <c r="F29" s="39"/>
       <c r="G29" s="39"/>
       <c r="H29" s="41"/>
-      <c r="I29" s="193"/>
-      <c r="J29" s="194"/>
+      <c r="I29" s="191"/>
+      <c r="J29" s="192"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1">
       <c r="A30" s="38"/>
@@ -6992,8 +7123,8 @@
       <c r="F30" s="39"/>
       <c r="G30" s="39"/>
       <c r="H30" s="41"/>
-      <c r="I30" s="193"/>
-      <c r="J30" s="194"/>
+      <c r="I30" s="191"/>
+      <c r="J30" s="192"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1">
       <c r="A31" s="38"/>
@@ -7004,8 +7135,8 @@
       <c r="F31" s="39"/>
       <c r="G31" s="39"/>
       <c r="H31" s="41"/>
-      <c r="I31" s="193"/>
-      <c r="J31" s="194"/>
+      <c r="I31" s="191"/>
+      <c r="J31" s="192"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1">
       <c r="A32" s="38"/>
@@ -7016,8 +7147,8 @@
       <c r="F32" s="39"/>
       <c r="G32" s="39"/>
       <c r="H32" s="41"/>
-      <c r="I32" s="193"/>
-      <c r="J32" s="194"/>
+      <c r="I32" s="191"/>
+      <c r="J32" s="192"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="38"/>
@@ -7028,8 +7159,8 @@
       <c r="F33" s="39"/>
       <c r="G33" s="39"/>
       <c r="H33" s="41"/>
-      <c r="I33" s="193"/>
-      <c r="J33" s="194"/>
+      <c r="I33" s="191"/>
+      <c r="J33" s="192"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="38"/>
@@ -7040,8 +7171,8 @@
       <c r="F34" s="39"/>
       <c r="G34" s="39"/>
       <c r="H34" s="41"/>
-      <c r="I34" s="193"/>
-      <c r="J34" s="194"/>
+      <c r="I34" s="191"/>
+      <c r="J34" s="192"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1">
       <c r="A35" s="38"/>
@@ -7052,8 +7183,8 @@
       <c r="F35" s="39"/>
       <c r="G35" s="39"/>
       <c r="H35" s="41"/>
-      <c r="I35" s="193"/>
-      <c r="J35" s="194"/>
+      <c r="I35" s="191"/>
+      <c r="J35" s="192"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1">
       <c r="A36" s="38"/>
@@ -7064,8 +7195,8 @@
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
       <c r="H36" s="41"/>
-      <c r="I36" s="193"/>
-      <c r="J36" s="194"/>
+      <c r="I36" s="191"/>
+      <c r="J36" s="192"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="A37" s="38"/>
@@ -7076,8 +7207,8 @@
       <c r="F37" s="39"/>
       <c r="G37" s="39"/>
       <c r="H37" s="41"/>
-      <c r="I37" s="193"/>
-      <c r="J37" s="194"/>
+      <c r="I37" s="191"/>
+      <c r="J37" s="192"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1">
       <c r="A38" s="38"/>
@@ -7088,8 +7219,8 @@
       <c r="F38" s="39"/>
       <c r="G38" s="39"/>
       <c r="H38" s="41"/>
-      <c r="I38" s="193"/>
-      <c r="J38" s="194"/>
+      <c r="I38" s="191"/>
+      <c r="J38" s="192"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1">
       <c r="A39" s="38"/>
@@ -7100,8 +7231,8 @@
       <c r="F39" s="39"/>
       <c r="G39" s="39"/>
       <c r="H39" s="41"/>
-      <c r="I39" s="193"/>
-      <c r="J39" s="194"/>
+      <c r="I39" s="191"/>
+      <c r="J39" s="192"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1">
       <c r="A40" s="38"/>
@@ -7112,8 +7243,8 @@
       <c r="F40" s="39"/>
       <c r="G40" s="39"/>
       <c r="H40" s="41"/>
-      <c r="I40" s="193"/>
-      <c r="J40" s="194"/>
+      <c r="I40" s="191"/>
+      <c r="J40" s="192"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
       <c r="A41" s="38"/>
@@ -7124,8 +7255,8 @@
       <c r="F41" s="39"/>
       <c r="G41" s="39"/>
       <c r="H41" s="41"/>
-      <c r="I41" s="193"/>
-      <c r="J41" s="194"/>
+      <c r="I41" s="191"/>
+      <c r="J41" s="192"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1">
       <c r="A42" s="38"/>
@@ -7136,8 +7267,8 @@
       <c r="F42" s="39"/>
       <c r="G42" s="39"/>
       <c r="H42" s="41"/>
-      <c r="I42" s="193"/>
-      <c r="J42" s="194"/>
+      <c r="I42" s="191"/>
+      <c r="J42" s="192"/>
     </row>
     <row r="43" spans="1:10" ht="12" customHeight="1">
       <c r="A43" s="38"/>
@@ -7148,8 +7279,8 @@
       <c r="F43" s="39"/>
       <c r="G43" s="39"/>
       <c r="H43" s="41"/>
-      <c r="I43" s="193"/>
-      <c r="J43" s="194"/>
+      <c r="I43" s="191"/>
+      <c r="J43" s="192"/>
     </row>
     <row r="44" spans="1:10" ht="12" customHeight="1">
       <c r="A44" s="38"/>
@@ -7160,8 +7291,8 @@
       <c r="F44" s="39"/>
       <c r="G44" s="39"/>
       <c r="H44" s="41"/>
-      <c r="I44" s="193"/>
-      <c r="J44" s="194"/>
+      <c r="I44" s="191"/>
+      <c r="J44" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -7189,10 +7320,10 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -7216,12 +7347,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
       <c r="E1" s="29" t="s">
         <v>1</v>
       </c>
@@ -7229,16 +7360,16 @@
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="G1" s="201" t="s">
+      <c r="G1" s="199" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="202"/>
-      <c r="I1" s="203" t="str">
+      <c r="H1" s="200"/>
+      <c r="I1" s="201" t="str">
         <f>'Update History'!F1</f>
         <v>CRMF2080</v>
       </c>
-      <c r="J1" s="204"/>
-      <c r="K1" s="205"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="203"/>
       <c r="L1" s="30" t="s">
         <v>5</v>
       </c>
@@ -7255,10 +7386,10 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="183"/>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
       <c r="E2" s="29" t="s">
         <v>2</v>
       </c>
@@ -7266,16 +7397,16 @@
         <f>'Update History'!D2</f>
         <v>ASOFT-CRM</v>
       </c>
-      <c r="G2" s="201" t="s">
+      <c r="G2" s="199" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="202"/>
-      <c r="I2" s="203" t="str">
+      <c r="H2" s="200"/>
+      <c r="I2" s="201" t="str">
         <f>'Update History'!F2</f>
         <v>Danh mục yêu cầu</v>
       </c>
-      <c r="J2" s="204"/>
-      <c r="K2" s="205"/>
+      <c r="J2" s="202"/>
+      <c r="K2" s="203"/>
       <c r="L2" s="30" t="s">
         <v>6</v>
       </c>
@@ -7441,10 +7572,10 @@
         <v>254</v>
       </c>
       <c r="E8" s="108" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F8" s="108" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G8" s="108" t="s">
         <v>156</v>
@@ -7511,7 +7642,7 @@
       <c r="C10" s="107">
         <v>5</v>
       </c>
-      <c r="D10" s="141" t="s">
+      <c r="D10" s="140" t="s">
         <v>257</v>
       </c>
       <c r="E10" s="108" t="s">
@@ -7587,7 +7718,7 @@
       <c r="C12" s="107">
         <v>7</v>
       </c>
-      <c r="D12" s="141" t="s">
+      <c r="D12" s="140" t="s">
         <v>258</v>
       </c>
       <c r="E12" s="108" t="s">
@@ -7893,7 +8024,7 @@
       <c r="C22" s="107">
         <v>17</v>
       </c>
-      <c r="D22" s="141" t="s">
+      <c r="D22" s="140" t="s">
         <v>166</v>
       </c>
       <c r="E22" s="120" t="s">
@@ -7930,7 +8061,7 @@
       <c r="C23" s="107">
         <v>18</v>
       </c>
-      <c r="D23" s="141" t="s">
+      <c r="D23" s="140" t="s">
         <v>167</v>
       </c>
       <c r="E23" s="120" t="s">
@@ -8167,14 +8298,14 @@
       <c r="C30" s="127">
         <v>19.600000000000001</v>
       </c>
-      <c r="D30" s="142" t="s">
-        <v>299</v>
+      <c r="D30" s="141" t="s">
+        <v>296</v>
       </c>
       <c r="E30" s="108" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F30" s="108" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G30" s="108" t="s">
         <v>176</v>
@@ -8202,7 +8333,7 @@
       <c r="C31" s="127">
         <v>19.7</v>
       </c>
-      <c r="D31" s="136" t="s">
+      <c r="D31" s="135" t="s">
         <v>233</v>
       </c>
       <c r="E31" s="108" t="s">
@@ -8237,7 +8368,7 @@
       <c r="C32" s="127">
         <v>19.8</v>
       </c>
-      <c r="D32" s="136" t="s">
+      <c r="D32" s="135" t="s">
         <v>258</v>
       </c>
       <c r="E32" s="108" t="s">
@@ -8272,7 +8403,7 @@
       <c r="C33" s="127">
         <v>19.899999999999999</v>
       </c>
-      <c r="D33" s="136" t="s">
+      <c r="D33" s="135" t="s">
         <v>260</v>
       </c>
       <c r="E33" s="108" t="s">
@@ -8299,22 +8430,40 @@
       <c r="N33" s="108"/>
       <c r="O33" s="108"/>
     </row>
-    <row r="34" spans="1:15" s="25" customFormat="1" ht="12.75">
-      <c r="A34" s="107"/>
-      <c r="B34" s="107"/>
-      <c r="C34" s="107"/>
-      <c r="D34" s="119"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="108"/>
-      <c r="G34" s="108"/>
-      <c r="H34" s="109"/>
-      <c r="I34" s="110"/>
-      <c r="J34" s="110"/>
-      <c r="K34" s="109"/>
-      <c r="L34" s="108"/>
-      <c r="M34" s="108"/>
-      <c r="N34" s="109"/>
-      <c r="O34" s="122"/>
+    <row r="34" spans="1:15" s="250" customFormat="1" ht="12.75">
+      <c r="A34" s="242">
+        <v>29</v>
+      </c>
+      <c r="B34" s="242" t="s">
+        <v>323</v>
+      </c>
+      <c r="C34" s="243">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="D34" s="244" t="s">
+        <v>321</v>
+      </c>
+      <c r="E34" s="245" t="s">
+        <v>322</v>
+      </c>
+      <c r="F34" s="245" t="s">
+        <v>322</v>
+      </c>
+      <c r="G34" s="246" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34" s="247" t="s">
+        <v>157</v>
+      </c>
+      <c r="I34" s="248"/>
+      <c r="J34" s="248"/>
+      <c r="K34" s="247" t="s">
+        <v>160</v>
+      </c>
+      <c r="L34" s="246"/>
+      <c r="M34" s="246"/>
+      <c r="N34" s="247"/>
+      <c r="O34" s="249"/>
     </row>
     <row r="35" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A35" s="107"/>
@@ -8369,7 +8518,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -8988,7 +9137,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="207" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="105"/>
@@ -9023,7 +9172,7 @@
       <c r="K1" s="46"/>
     </row>
     <row r="2" spans="1:11" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="210"/>
+      <c r="A2" s="208"/>
       <c r="B2" s="106"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
@@ -9071,15 +9220,15 @@
       <c r="E4" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="183" t="s">
+      <c r="F4" s="174" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="183"/>
-      <c r="H4" s="183" t="s">
+      <c r="G4" s="174"/>
+      <c r="H4" s="174" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="183"/>
-      <c r="J4" s="183"/>
+      <c r="I4" s="174"/>
+      <c r="J4" s="174"/>
     </row>
     <row r="5" spans="1:11" s="117" customFormat="1" ht="30.75" customHeight="1">
       <c r="A5" s="114">
@@ -9095,13 +9244,13 @@
       <c r="E5" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="211" t="s">
+      <c r="F5" s="209" t="s">
         <v>269</v>
       </c>
-      <c r="G5" s="212"/>
-      <c r="H5" s="212"/>
-      <c r="I5" s="213"/>
-      <c r="J5" s="211" t="s">
+      <c r="G5" s="210"/>
+      <c r="H5" s="210"/>
+      <c r="I5" s="211"/>
+      <c r="J5" s="209" t="s">
         <v>267</v>
       </c>
     </row>
@@ -9119,11 +9268,11 @@
       <c r="E6" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="F6" s="214"/>
-      <c r="G6" s="215"/>
-      <c r="H6" s="215"/>
-      <c r="I6" s="216"/>
-      <c r="J6" s="214"/>
+      <c r="F6" s="212"/>
+      <c r="G6" s="213"/>
+      <c r="H6" s="213"/>
+      <c r="I6" s="214"/>
+      <c r="J6" s="212"/>
     </row>
     <row r="7" spans="1:11" s="117" customFormat="1" ht="45.75" customHeight="1">
       <c r="A7" s="114">
@@ -9139,12 +9288,12 @@
       <c r="E7" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="206" t="s">
+      <c r="F7" s="204" t="s">
         <v>270</v>
       </c>
-      <c r="G7" s="207"/>
-      <c r="H7" s="207"/>
-      <c r="I7" s="208"/>
+      <c r="G7" s="205"/>
+      <c r="H7" s="205"/>
+      <c r="I7" s="206"/>
       <c r="J7" s="116" t="s">
         <v>190</v>
       </c>
@@ -9163,12 +9312,12 @@
       <c r="E8" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="206" t="s">
+      <c r="F8" s="204" t="s">
         <v>239</v>
       </c>
-      <c r="G8" s="207"/>
-      <c r="H8" s="207"/>
-      <c r="I8" s="208"/>
+      <c r="G8" s="205"/>
+      <c r="H8" s="205"/>
+      <c r="I8" s="206"/>
       <c r="J8" s="116" t="s">
         <v>240</v>
       </c>
@@ -9187,12 +9336,12 @@
       <c r="E9" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="F9" s="206" t="s">
+      <c r="F9" s="204" t="s">
         <v>271</v>
       </c>
-      <c r="G9" s="207"/>
-      <c r="H9" s="207"/>
-      <c r="I9" s="208"/>
+      <c r="G9" s="205"/>
+      <c r="H9" s="205"/>
+      <c r="I9" s="206"/>
       <c r="J9" s="116" t="s">
         <v>241</v>
       </c>
@@ -9225,8 +9374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1048216"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:J8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D10" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -9252,20 +9401,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
       <c r="E1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="229" t="str">
+      <c r="F1" s="215" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="G1" s="229"/>
+      <c r="G1" s="215"/>
       <c r="H1" s="26" t="s">
         <v>3</v>
       </c>
@@ -9283,28 +9432,28 @@
       <c r="L1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="217" t="str">
+      <c r="M1" s="222" t="str">
         <f>'Update History'!J1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="N1" s="218"/>
-      <c r="O1" s="219"/>
+      <c r="N1" s="223"/>
+      <c r="O1" s="224"/>
       <c r="P1" s="46"/>
       <c r="Q1" s="46"/>
     </row>
     <row r="2" spans="1:17" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="183"/>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
       <c r="E2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="229" t="str">
+      <c r="F2" s="215" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT-CRM</v>
       </c>
-      <c r="G2" s="229"/>
+      <c r="G2" s="215"/>
       <c r="H2" s="26" t="s">
         <v>49</v>
       </c>
@@ -9322,12 +9471,12 @@
       <c r="L2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="217" t="str">
+      <c r="M2" s="222" t="str">
         <f>'Update History'!J2</f>
         <v>25/03/2017</v>
       </c>
-      <c r="N2" s="218"/>
-      <c r="O2" s="219"/>
+      <c r="N2" s="223"/>
+      <c r="O2" s="224"/>
       <c r="P2" s="46"/>
       <c r="Q2" s="46"/>
     </row>
@@ -9350,12 +9499,12 @@
       <c r="F4" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="188" t="s">
+      <c r="G4" s="186" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="190"/>
-      <c r="I4" s="190"/>
-      <c r="J4" s="189"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="187"/>
       <c r="K4" s="35" t="s">
         <v>56</v>
       </c>
@@ -9391,12 +9540,12 @@
       <c r="F5" s="130" t="s">
         <v>199</v>
       </c>
-      <c r="G5" s="223" t="s">
+      <c r="G5" s="216" t="s">
         <v>217</v>
       </c>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
-      <c r="J5" s="225"/>
+      <c r="H5" s="217"/>
+      <c r="I5" s="217"/>
+      <c r="J5" s="218"/>
       <c r="K5" s="122" t="s">
         <v>198</v>
       </c>
@@ -9434,12 +9583,12 @@
       <c r="F6" s="130" t="s">
         <v>201</v>
       </c>
-      <c r="G6" s="226" t="s">
+      <c r="G6" s="225" t="s">
         <v>219</v>
       </c>
-      <c r="H6" s="227"/>
-      <c r="I6" s="227"/>
-      <c r="J6" s="228"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
+      <c r="J6" s="227"/>
       <c r="K6" s="122" t="s">
         <v>194</v>
       </c>
@@ -9477,12 +9626,12 @@
       <c r="F7" s="130" t="s">
         <v>200</v>
       </c>
-      <c r="G7" s="226" t="s">
+      <c r="G7" s="225" t="s">
         <v>219</v>
       </c>
-      <c r="H7" s="227"/>
-      <c r="I7" s="227"/>
-      <c r="J7" s="228"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="227"/>
       <c r="K7" s="122" t="s">
         <v>194</v>
       </c>
@@ -9501,46 +9650,46 @@
       <c r="P7" s="46"/>
       <c r="Q7" s="46"/>
     </row>
-    <row r="8" spans="1:17" s="153" customFormat="1" ht="123.75">
-      <c r="A8" s="145">
+    <row r="8" spans="1:17" s="151" customFormat="1" ht="135">
+      <c r="A8" s="144">
         <v>5</v>
       </c>
-      <c r="B8" s="145" t="s">
+      <c r="B8" s="144" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="146"/>
-      <c r="D8" s="147" t="s">
+      <c r="C8" s="145"/>
+      <c r="D8" s="146" t="s">
         <v>191</v>
       </c>
-      <c r="E8" s="147" t="s">
+      <c r="E8" s="146" t="s">
         <v>195</v>
       </c>
-      <c r="F8" s="148" t="s">
+      <c r="F8" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="G8" s="230" t="s">
-        <v>320</v>
-      </c>
-      <c r="H8" s="231"/>
-      <c r="I8" s="231"/>
-      <c r="J8" s="232"/>
-      <c r="K8" s="149" t="s">
-        <v>321</v>
-      </c>
-      <c r="L8" s="149" t="s">
-        <v>322</v>
-      </c>
-      <c r="M8" s="150" t="s">
+      <c r="G8" s="251" t="s">
+        <v>324</v>
+      </c>
+      <c r="H8" s="252"/>
+      <c r="I8" s="252"/>
+      <c r="J8" s="253"/>
+      <c r="K8" s="254" t="s">
+        <v>325</v>
+      </c>
+      <c r="L8" s="254" t="s">
+        <v>326</v>
+      </c>
+      <c r="M8" s="148" t="s">
         <v>222</v>
       </c>
-      <c r="N8" s="151" t="s">
+      <c r="N8" s="149" t="s">
         <v>196</v>
       </c>
-      <c r="O8" s="150" t="s">
+      <c r="O8" s="148" t="s">
         <v>223</v>
       </c>
-      <c r="P8" s="152"/>
-      <c r="Q8" s="152"/>
+      <c r="P8" s="150"/>
+      <c r="Q8" s="150"/>
     </row>
     <row r="9" spans="1:17" s="25" customFormat="1" ht="87.75" customHeight="1">
       <c r="A9" s="107">
@@ -9559,17 +9708,17 @@
       <c r="F9" s="130" t="s">
         <v>203</v>
       </c>
-      <c r="G9" s="233" t="s">
+      <c r="G9" s="219" t="s">
         <v>273</v>
       </c>
-      <c r="H9" s="234"/>
-      <c r="I9" s="234"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="133" t="s">
+      <c r="H9" s="220"/>
+      <c r="I9" s="220"/>
+      <c r="J9" s="221"/>
+      <c r="K9" s="132" t="s">
         <v>272</v>
       </c>
-      <c r="L9" s="133" t="s">
-        <v>301</v>
+      <c r="L9" s="132" t="s">
+        <v>298</v>
       </c>
       <c r="M9" s="67" t="s">
         <v>224</v>
@@ -9600,17 +9749,17 @@
       <c r="F10" s="130" t="s">
         <v>204</v>
       </c>
-      <c r="G10" s="220" t="s">
-        <v>295</v>
-      </c>
-      <c r="H10" s="221"/>
-      <c r="I10" s="221"/>
-      <c r="J10" s="222"/>
-      <c r="K10" s="132" t="s">
-        <v>296</v>
-      </c>
-      <c r="L10" s="132" t="s">
-        <v>297</v>
+      <c r="G10" s="251" t="s">
+        <v>327</v>
+      </c>
+      <c r="H10" s="252"/>
+      <c r="I10" s="252"/>
+      <c r="J10" s="253"/>
+      <c r="K10" s="254" t="s">
+        <v>328</v>
+      </c>
+      <c r="L10" s="254" t="s">
+        <v>329</v>
       </c>
       <c r="M10" s="67"/>
       <c r="N10" s="131" t="s">
@@ -9639,20 +9788,20 @@
       <c r="F11" s="130" t="s">
         <v>226</v>
       </c>
-      <c r="G11" s="223" t="s">
+      <c r="G11" s="216" t="s">
         <v>229</v>
       </c>
-      <c r="H11" s="224"/>
-      <c r="I11" s="224"/>
-      <c r="J11" s="225"/>
+      <c r="H11" s="217"/>
+      <c r="I11" s="217"/>
+      <c r="J11" s="218"/>
       <c r="K11" s="118" t="s">
         <v>198</v>
       </c>
       <c r="L11" s="118" t="s">
         <v>205</v>
       </c>
-      <c r="M11" s="134"/>
-      <c r="N11" s="135" t="s">
+      <c r="M11" s="133"/>
+      <c r="N11" s="134" t="s">
         <v>193</v>
       </c>
       <c r="O11" s="67" t="s">
@@ -9678,22 +9827,22 @@
       <c r="F12" s="130" t="s">
         <v>227</v>
       </c>
-      <c r="G12" s="220" t="s">
-        <v>295</v>
-      </c>
-      <c r="H12" s="221"/>
-      <c r="I12" s="221"/>
-      <c r="J12" s="222"/>
-      <c r="K12" s="132" t="s">
-        <v>296</v>
-      </c>
-      <c r="L12" s="132" t="s">
-        <v>297</v>
+      <c r="G12" s="251" t="s">
+        <v>327</v>
+      </c>
+      <c r="H12" s="252"/>
+      <c r="I12" s="252"/>
+      <c r="J12" s="253"/>
+      <c r="K12" s="254" t="s">
+        <v>330</v>
+      </c>
+      <c r="L12" s="254" t="s">
+        <v>329</v>
       </c>
       <c r="M12" s="67" t="s">
         <v>231</v>
       </c>
-      <c r="N12" s="135" t="s">
+      <c r="N12" s="134" t="s">
         <v>193</v>
       </c>
       <c r="O12" s="126" t="s">
@@ -9708,6 +9857,12 @@
   </sheetData>
   <dataConsolidate link="1"/>
   <mergeCells count="14">
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
@@ -9716,12 +9871,6 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="G9:J9"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="M1048216:M1048576 M11 M5:M6"/>
@@ -9750,8 +9899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A31" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -9767,10 +9916,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="183"/>
+      <c r="B1" s="174"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -9801,8 +9950,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="183"/>
-      <c r="B2" s="183"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="174"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -10006,22 +10155,22 @@
     <row r="18" spans="1:10" ht="12" customHeight="1">
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
-      <c r="D18" s="137"/>
-      <c r="E18" s="137"/>
-      <c r="F18" s="137"/>
-      <c r="G18" s="137"/>
-      <c r="H18" s="137"/>
+      <c r="D18" s="136"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="136"/>
+      <c r="G18" s="136"/>
+      <c r="H18" s="136"/>
       <c r="I18" s="39"/>
       <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1">
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
-      <c r="D19" s="137"/>
-      <c r="E19" s="137"/>
-      <c r="F19" s="137"/>
-      <c r="G19" s="137"/>
-      <c r="H19" s="137"/>
+      <c r="D19" s="136"/>
+      <c r="E19" s="136"/>
+      <c r="F19" s="136"/>
+      <c r="G19" s="136"/>
+      <c r="H19" s="136"/>
       <c r="I19" s="39"/>
       <c r="J19" s="42"/>
     </row>
@@ -10040,16 +10189,16 @@
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
       <c r="B21" s="39"/>
-      <c r="C21" s="236" t="s">
+      <c r="C21" s="228" t="s">
         <v>281</v>
       </c>
-      <c r="D21" s="237"/>
-      <c r="E21" s="237"/>
-      <c r="F21" s="237"/>
-      <c r="G21" s="237"/>
-      <c r="H21" s="237"/>
-      <c r="I21" s="237"/>
-      <c r="J21" s="237"/>
+      <c r="D21" s="229"/>
+      <c r="E21" s="229"/>
+      <c r="F21" s="229"/>
+      <c r="G21" s="229"/>
+      <c r="H21" s="229"/>
+      <c r="I21" s="229"/>
+      <c r="J21" s="229"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="B22" s="39"/>
@@ -10202,28 +10351,28 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
-      <c r="C34" s="138" t="s">
+      <c r="C34" s="137" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1">
-      <c r="C35" s="138" t="s">
+      <c r="C35" s="137" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="28.5" customHeight="1">
       <c r="A36" s="61"/>
       <c r="B36" s="39"/>
-      <c r="C36" s="238" t="s">
+      <c r="C36" s="230" t="s">
         <v>236</v>
       </c>
-      <c r="D36" s="238"/>
-      <c r="E36" s="238"/>
-      <c r="F36" s="238"/>
-      <c r="G36" s="238"/>
-      <c r="H36" s="238"/>
-      <c r="I36" s="238"/>
-      <c r="J36" s="238"/>
+      <c r="D36" s="230"/>
+      <c r="E36" s="230"/>
+      <c r="F36" s="230"/>
+      <c r="G36" s="230"/>
+      <c r="H36" s="230"/>
+      <c r="I36" s="230"/>
+      <c r="J36" s="230"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="A37" s="38"/>
@@ -10351,13 +10500,13 @@
     </row>
     <row r="47" spans="1:10" ht="12" customHeight="1">
       <c r="B47" s="39"/>
-      <c r="C47" s="239"/>
-      <c r="D47" s="239"/>
-      <c r="E47" s="239"/>
-      <c r="F47" s="239"/>
-      <c r="G47" s="239"/>
-      <c r="H47" s="239"/>
-      <c r="I47" s="239"/>
+      <c r="C47" s="231"/>
+      <c r="D47" s="231"/>
+      <c r="E47" s="231"/>
+      <c r="F47" s="231"/>
+      <c r="G47" s="231"/>
+      <c r="H47" s="231"/>
+      <c r="I47" s="231"/>
       <c r="J47" s="42"/>
     </row>
     <row r="48" spans="1:10" ht="12" customHeight="1">
@@ -10416,45 +10565,45 @@
       <c r="C52" s="39" t="s">
         <v>291</v>
       </c>
-      <c r="D52" s="140"/>
-      <c r="E52" s="140"/>
-      <c r="F52" s="140"/>
-      <c r="G52" s="140"/>
-      <c r="H52" s="140"/>
-      <c r="I52" s="140"/>
+      <c r="D52" s="139"/>
+      <c r="E52" s="139"/>
+      <c r="F52" s="139"/>
+      <c r="G52" s="139"/>
+      <c r="H52" s="139"/>
+      <c r="I52" s="139"/>
       <c r="J52" s="42"/>
     </row>
     <row r="53" spans="1:10" ht="12" customHeight="1">
       <c r="B53" s="66"/>
-      <c r="C53" s="140"/>
-      <c r="D53" s="140"/>
-      <c r="E53" s="140"/>
-      <c r="F53" s="140"/>
-      <c r="G53" s="140"/>
-      <c r="H53" s="140"/>
-      <c r="I53" s="140"/>
+      <c r="C53" s="139"/>
+      <c r="D53" s="139"/>
+      <c r="E53" s="139"/>
+      <c r="F53" s="139"/>
+      <c r="G53" s="139"/>
+      <c r="H53" s="139"/>
+      <c r="I53" s="139"/>
       <c r="J53" s="42"/>
     </row>
     <row r="54" spans="1:10" ht="12" customHeight="1">
       <c r="B54" s="66"/>
-      <c r="C54" s="140"/>
-      <c r="D54" s="140"/>
-      <c r="E54" s="140"/>
-      <c r="F54" s="140"/>
-      <c r="G54" s="140"/>
-      <c r="H54" s="140"/>
-      <c r="I54" s="140"/>
+      <c r="C54" s="139"/>
+      <c r="D54" s="139"/>
+      <c r="E54" s="139"/>
+      <c r="F54" s="139"/>
+      <c r="G54" s="139"/>
+      <c r="H54" s="139"/>
+      <c r="I54" s="139"/>
       <c r="J54" s="42"/>
     </row>
     <row r="55" spans="1:10" ht="12" customHeight="1">
       <c r="B55" s="66"/>
-      <c r="C55" s="140"/>
-      <c r="D55" s="140"/>
-      <c r="E55" s="140"/>
-      <c r="F55" s="140"/>
-      <c r="G55" s="140"/>
-      <c r="H55" s="140"/>
-      <c r="I55" s="140"/>
+      <c r="C55" s="139"/>
+      <c r="D55" s="139"/>
+      <c r="E55" s="139"/>
+      <c r="F55" s="139"/>
+      <c r="G55" s="139"/>
+      <c r="H55" s="139"/>
+      <c r="I55" s="139"/>
       <c r="J55" s="42"/>
     </row>
     <row r="56" spans="1:10" ht="12" customHeight="1">
@@ -10472,15 +10621,15 @@
     </row>
     <row r="57" spans="1:10" ht="12" customHeight="1">
       <c r="B57" s="66"/>
-      <c r="C57" s="139" t="s">
+      <c r="C57" s="138" t="s">
         <v>292</v>
       </c>
-      <c r="D57" s="139"/>
-      <c r="E57" s="139"/>
-      <c r="F57" s="139"/>
-      <c r="G57" s="139"/>
-      <c r="H57" s="139"/>
-      <c r="I57" s="139"/>
+      <c r="D57" s="138"/>
+      <c r="E57" s="138"/>
+      <c r="F57" s="138"/>
+      <c r="G57" s="138"/>
+      <c r="H57" s="138"/>
+      <c r="I57" s="138"/>
       <c r="J57" s="42"/>
     </row>
     <row r="58" spans="1:10" ht="12" customHeight="1">
@@ -11000,10 +11149,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="183"/>
+      <c r="B1" s="174"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -11034,8 +11183,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="183"/>
-      <c r="B2" s="183"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="174"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Update sau Review lần 1
</commit_message>
<xml_diff>
--- a/2018/CRM/03_DetailDesign/CRMF2080_Danh muc yeu cau.xlsx
+++ b/2018/CRM/03_DetailDesign/CRMF2080_Danh muc yeu cau.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Coverpage" sheetId="20" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Item Screen'!$A$4:$P$36</definedName>
     <definedName name="CNT">#REF!</definedName>
     <definedName name="_xlnm.Criteria">#REF!</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
@@ -45,11 +46,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="10">'Code Standar'!$A$1:$C$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Coverpage!$A$1:$J$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Data Definition'!$A$1:$J$18</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'Data Input'!$A$1:$O$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Data Input'!$A$1:$P$45</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'Form Func Spec'!$A$1:$J$81</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">'Func Spec'!$A$1:$J$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="9">Help!$A$1:$K$62</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Item Screen'!$A$1:$O$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Item Screen'!$A$1:$P$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Layout Screen'!$A$1:$J$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Update History'!$A$1:$J$34</definedName>
     <definedName name="RB">#REF!</definedName>
@@ -407,7 +408,7 @@
     <author>vinhphong</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -421,7 +422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="1" shapeId="0">
+    <comment ref="E4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -434,7 +435,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="1" shapeId="0">
+    <comment ref="F4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -447,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0">
+    <comment ref="G4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -460,7 +461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="1" shapeId="0">
+    <comment ref="H4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -486,7 +487,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="1" shapeId="0">
+    <comment ref="I4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -503,7 +504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="1" shapeId="0">
+    <comment ref="J4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -516,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="0" shapeId="0">
+    <comment ref="K4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -530,7 +531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K4" authorId="1" shapeId="0">
+    <comment ref="L4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -622,7 +623,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L4" authorId="1" shapeId="0">
+    <comment ref="M4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -657,7 +658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0" shapeId="0">
+    <comment ref="N4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -673,7 +674,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N4" authorId="1" shapeId="0">
+    <comment ref="O4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -821,7 +822,7 @@
     <author>Le Thi Thu Hien</author>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -838,7 +839,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -853,7 +854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="G4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -871,7 +872,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0">
+    <comment ref="H4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -885,7 +886,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K4" authorId="0" shapeId="0">
+    <comment ref="L4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -899,7 +900,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L4" authorId="0" shapeId="0">
+    <comment ref="M4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -913,7 +914,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N4" authorId="1" shapeId="0">
+    <comment ref="O4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1333,7 +1334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="334">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2534,7 +2535,21 @@
     <t>RequestTypeID</t>
   </si>
   <si>
-    <t>Ver 2.0</t>
+    <t xml:space="preserve">- STT yêu cầu là: 4 (bên file Tasklist)
+Bổ sung trường Loại yêu cầu </t>
+  </si>
+  <si>
+    <t>Ver 3.0</t>
+  </si>
+  <si>
+    <t>Loại Bug</t>
+  </si>
+  <si>
+    <t>BugTypeID</t>
+  </si>
+  <si>
+    <t>- Combo hiển thị 1 cột: @Description as BugTypeName
+- Chọn giá trị Fill giá trị lên Combo: BugTypeName</t>
   </si>
   <si>
     <t xml:space="preserve">EXEC CRMP20801 ( 
@@ -2549,8 +2564,12 @@
   @ConditionRequestID Nvarchar(max), 
   @PageNumber INT,
   @PageSize INT,
-  @RequestTypeID
+  @RequestTypeID ,
+  @BugTypeID
 ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizeindex  </t>
   </si>
   <si>
     <t xml:space="preserve">   @DivisionID   
@@ -2564,7 +2583,8 @@
 @ConditionRequestID
   @PageNumber 
   @PageSize 
-  @RequestTypeID</t>
+  @RequestTypeID
+  @BugTypeID</t>
   </si>
   <si>
     <t xml:space="preserve"> Biến môi trường   
@@ -2578,7 +2598,8 @@
 @ConditionRequestID 
   @PageNumber 
   @PageSize 
-  @RequestTypeID</t>
+  @RequestTypeID
+  @BugtypeID</t>
   </si>
   <si>
     <t xml:space="preserve">EXEC CRMP20803 ( 
@@ -2590,7 +2611,8 @@
   @RequestStatus nvarchar(250),
   @PriorityID nvarchar(100),
   @UserID  VARCHAR(50),
-  @RequestTypeID nvarchar(250)
+  @RequestTypeID varchar(250),
+  @BugTypeID varchar(50)
 ) </t>
   </si>
   <si>
@@ -2602,7 +2624,8 @@
   @RequestStatus 
   @PriorityID 
   @UserID 
-  @RequestTypeID</t>
+  @RequestTypeID
+  @BugTypeID</t>
   </si>
   <si>
     <t xml:space="preserve"> Biến môi trường   
@@ -2613,22 +2636,8 @@
   @RequestStatus 
   @PriorityID 
   Biến môi trường  
-  @RequestTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   @DivisionID   
-  @DivisionIDList      
-  @RequestSubject 
-  @AccountID 
-  @AssignedToUserID 
-  @RequestStatus 
-  @PriorityID 
-  @UserID  
-  @RequestTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- STT yêu cầu là: 4 (bên file Tasklist)
-Bổ sung trường Loại yêu cầu </t>
+  @RequestTypeID
+  @BugTypeID</t>
   </si>
 </sst>
 </file>
@@ -3545,9 +3554,6 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3572,6 +3578,9 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="11" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3650,6 +3659,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3837,9 +3849,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3984,19 +3993,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2543175</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>2514600</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4016,8 +4025,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="762000"/>
-          <a:ext cx="9696450" cy="5867400"/>
+          <a:off x="47625" y="638175"/>
+          <a:ext cx="9620250" cy="6781800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5470,14 +5479,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14.25">
-      <c r="B1" s="250" t="s">
+      <c r="B1" s="251" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
+      <c r="C1" s="251"/>
+      <c r="D1" s="251"/>
+      <c r="E1" s="251"/>
+      <c r="F1" s="251"/>
+      <c r="G1" s="251"/>
     </row>
     <row r="2" spans="2:7" s="17" customFormat="1">
       <c r="B2" s="16"/>
@@ -5670,11 +5679,11 @@
       </c>
     </row>
     <row r="27" spans="2:10" ht="200.25" customHeight="1">
-      <c r="E27" s="251" t="s">
+      <c r="E27" s="252" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="252"/>
-      <c r="G27" s="253"/>
+      <c r="F27" s="253"/>
+      <c r="G27" s="254"/>
     </row>
     <row r="28" spans="2:10">
       <c r="J28" s="152"/>
@@ -6056,8 +6065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:J8"/>
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -6073,10 +6082,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="197" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
+      <c r="B1" s="197"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -6099,12 +6108,12 @@
         <v>7</v>
       </c>
       <c r="J1" s="80" t="s">
-        <v>208</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
+      <c r="A2" s="197"/>
+      <c r="B2" s="197"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -6127,7 +6136,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="81" t="s">
-        <v>245</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1">
@@ -6143,14 +6152,14 @@
       <c r="D4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="197" t="s">
+      <c r="E4" s="198" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="197"/>
-      <c r="G4" s="197"/>
-      <c r="H4" s="197"/>
-      <c r="I4" s="197"/>
-      <c r="J4" s="197"/>
+      <c r="F4" s="198"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
+      <c r="J4" s="198"/>
     </row>
     <row r="5" spans="1:10" ht="24.75" customHeight="1">
       <c r="A5" s="36">
@@ -6187,14 +6196,14 @@
       <c r="D6" s="143">
         <v>42860</v>
       </c>
-      <c r="E6" s="198" t="s">
+      <c r="E6" s="199" t="s">
         <v>317</v>
       </c>
-      <c r="F6" s="199"/>
-      <c r="G6" s="199"/>
-      <c r="H6" s="199"/>
-      <c r="I6" s="199"/>
-      <c r="J6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="200"/>
+      <c r="H6" s="200"/>
+      <c r="I6" s="200"/>
+      <c r="J6" s="201"/>
     </row>
     <row r="7" spans="1:10" ht="27.75" customHeight="1">
       <c r="A7" s="72">
@@ -6209,14 +6218,14 @@
       <c r="D7" s="154" t="s">
         <v>319</v>
       </c>
-      <c r="E7" s="254" t="s">
-        <v>330</v>
-      </c>
-      <c r="F7" s="191"/>
-      <c r="G7" s="191"/>
-      <c r="H7" s="191"/>
-      <c r="I7" s="191"/>
-      <c r="J7" s="192"/>
+      <c r="E7" s="191" t="s">
+        <v>322</v>
+      </c>
+      <c r="F7" s="192"/>
+      <c r="G7" s="192"/>
+      <c r="H7" s="192"/>
+      <c r="I7" s="192"/>
+      <c r="J7" s="193"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
       <c r="A8" s="73">
@@ -6227,12 +6236,12 @@
       </c>
       <c r="C8" s="65"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="193"/>
-      <c r="F8" s="194"/>
-      <c r="G8" s="194"/>
-      <c r="H8" s="194"/>
-      <c r="I8" s="194"/>
-      <c r="J8" s="195"/>
+      <c r="E8" s="194"/>
+      <c r="F8" s="195"/>
+      <c r="G8" s="195"/>
+      <c r="H8" s="195"/>
+      <c r="I8" s="195"/>
+      <c r="J8" s="196"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
       <c r="A9" s="74">
@@ -6728,10 +6737,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="197" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
+      <c r="B1" s="197"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -6758,12 +6767,12 @@
       </c>
       <c r="J1" s="57" t="str">
         <f>'Update History'!J1</f>
-        <v>Thị Phượng</v>
+        <v>Tấn Đạt</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
+      <c r="A2" s="197"/>
+      <c r="B2" s="197"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -6790,24 +6799,24 @@
       </c>
       <c r="J2" s="57" t="str">
         <f>'Update History'!J2</f>
-        <v>25/03/2017</v>
+        <v>26/01/2018</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="202" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="203"/>
-      <c r="C4" s="203"/>
-      <c r="D4" s="203"/>
-      <c r="E4" s="203"/>
-      <c r="F4" s="203"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="202"/>
-      <c r="I4" s="201" t="s">
+      <c r="B4" s="204"/>
+      <c r="C4" s="204"/>
+      <c r="D4" s="204"/>
+      <c r="E4" s="204"/>
+      <c r="F4" s="204"/>
+      <c r="G4" s="204"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="202" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="202"/>
+      <c r="J4" s="203"/>
     </row>
     <row r="5" spans="1:10" ht="12" customHeight="1">
       <c r="A5"/>
@@ -6818,10 +6827,10 @@
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
       <c r="H5" s="40"/>
-      <c r="I5" s="208" t="s">
+      <c r="I5" s="209" t="s">
         <v>247</v>
       </c>
-      <c r="J5" s="209"/>
+      <c r="J5" s="210"/>
     </row>
     <row r="6" spans="1:10" ht="12" customHeight="1">
       <c r="A6" s="38"/>
@@ -6832,8 +6841,8 @@
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
       <c r="H6" s="41"/>
-      <c r="I6" s="210"/>
-      <c r="J6" s="211"/>
+      <c r="I6" s="211"/>
+      <c r="J6" s="212"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1">
       <c r="A7" s="38"/>
@@ -6844,8 +6853,8 @@
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
       <c r="H7" s="41"/>
-      <c r="I7" s="210"/>
-      <c r="J7" s="211"/>
+      <c r="I7" s="211"/>
+      <c r="J7" s="212"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
       <c r="A8" s="38"/>
@@ -6856,8 +6865,8 @@
       <c r="F8" s="39"/>
       <c r="G8" s="39"/>
       <c r="H8" s="41"/>
-      <c r="I8" s="210"/>
-      <c r="J8" s="211"/>
+      <c r="I8" s="211"/>
+      <c r="J8" s="212"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
       <c r="A9" s="38"/>
@@ -6868,8 +6877,8 @@
       <c r="F9" s="39"/>
       <c r="G9" s="39"/>
       <c r="H9" s="41"/>
-      <c r="I9" s="210"/>
-      <c r="J9" s="211"/>
+      <c r="I9" s="211"/>
+      <c r="J9" s="212"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1">
       <c r="A10" s="38"/>
@@ -6880,8 +6889,8 @@
       <c r="F10" s="39"/>
       <c r="G10" s="39"/>
       <c r="H10" s="41"/>
-      <c r="I10" s="212"/>
-      <c r="J10" s="213"/>
+      <c r="I10" s="213"/>
+      <c r="J10" s="214"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
       <c r="A11" s="38"/>
@@ -6892,10 +6901,10 @@
       <c r="F11" s="39"/>
       <c r="G11" s="39"/>
       <c r="H11" s="42"/>
-      <c r="I11" s="201" t="s">
+      <c r="I11" s="202" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="202"/>
+      <c r="J11" s="203"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1">
       <c r="A12" s="38"/>
@@ -6906,10 +6915,10 @@
       <c r="F12" s="39"/>
       <c r="G12" s="39"/>
       <c r="H12" s="41"/>
-      <c r="I12" s="204" t="s">
+      <c r="I12" s="205" t="s">
         <v>248</v>
       </c>
-      <c r="J12" s="205"/>
+      <c r="J12" s="206"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
       <c r="A13" s="38"/>
@@ -6920,8 +6929,8 @@
       <c r="F13" s="39"/>
       <c r="G13" s="39"/>
       <c r="H13" s="41"/>
-      <c r="I13" s="206"/>
-      <c r="J13" s="207"/>
+      <c r="I13" s="207"/>
+      <c r="J13" s="208"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
       <c r="A14" s="38"/>
@@ -6932,8 +6941,8 @@
       <c r="F14" s="39"/>
       <c r="G14" s="39"/>
       <c r="H14" s="41"/>
-      <c r="I14" s="206"/>
-      <c r="J14" s="207"/>
+      <c r="I14" s="207"/>
+      <c r="J14" s="208"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
       <c r="A15" s="38"/>
@@ -6944,8 +6953,8 @@
       <c r="F15" s="39"/>
       <c r="G15" s="39"/>
       <c r="H15" s="41"/>
-      <c r="I15" s="206"/>
-      <c r="J15" s="207"/>
+      <c r="I15" s="207"/>
+      <c r="J15" s="208"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
       <c r="A16" s="38"/>
@@ -6956,8 +6965,8 @@
       <c r="F16" s="39"/>
       <c r="G16" s="39"/>
       <c r="H16" s="41"/>
-      <c r="I16" s="206"/>
-      <c r="J16" s="207"/>
+      <c r="I16" s="207"/>
+      <c r="J16" s="208"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1">
       <c r="A17" s="38"/>
@@ -6968,8 +6977,8 @@
       <c r="F17" s="39"/>
       <c r="G17" s="39"/>
       <c r="H17" s="41"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="207"/>
+      <c r="I17" s="207"/>
+      <c r="J17" s="208"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1">
       <c r="A18" s="38"/>
@@ -6980,8 +6989,8 @@
       <c r="F18" s="39"/>
       <c r="G18" s="39"/>
       <c r="H18" s="41"/>
-      <c r="I18" s="206"/>
-      <c r="J18" s="207"/>
+      <c r="I18" s="207"/>
+      <c r="J18" s="208"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1">
       <c r="A19" s="38"/>
@@ -6992,8 +7001,8 @@
       <c r="F19" s="39"/>
       <c r="G19" s="39"/>
       <c r="H19" s="41"/>
-      <c r="I19" s="206"/>
-      <c r="J19" s="207"/>
+      <c r="I19" s="207"/>
+      <c r="J19" s="208"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1">
       <c r="A20" s="38"/>
@@ -7004,8 +7013,8 @@
       <c r="F20" s="39"/>
       <c r="G20" s="39"/>
       <c r="H20" s="41"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="207"/>
+      <c r="I20" s="207"/>
+      <c r="J20" s="208"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
       <c r="A21" s="38"/>
@@ -7016,8 +7025,8 @@
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
       <c r="H21" s="41"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="207"/>
+      <c r="I21" s="207"/>
+      <c r="J21" s="208"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="A22" s="38"/>
@@ -7028,8 +7037,8 @@
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
       <c r="H22" s="41"/>
-      <c r="I22" s="206"/>
-      <c r="J22" s="207"/>
+      <c r="I22" s="207"/>
+      <c r="J22" s="208"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1">
       <c r="A23" s="38"/>
@@ -7040,8 +7049,8 @@
       <c r="F23" s="39"/>
       <c r="G23" s="39"/>
       <c r="H23" s="41"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="207"/>
+      <c r="I23" s="207"/>
+      <c r="J23" s="208"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1">
       <c r="A24" s="38"/>
@@ -7052,8 +7061,8 @@
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
       <c r="H24" s="41"/>
-      <c r="I24" s="206"/>
-      <c r="J24" s="207"/>
+      <c r="I24" s="207"/>
+      <c r="J24" s="208"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1">
       <c r="A25" s="38"/>
@@ -7064,8 +7073,8 @@
       <c r="F25" s="39"/>
       <c r="G25" s="39"/>
       <c r="H25" s="41"/>
-      <c r="I25" s="206"/>
-      <c r="J25" s="207"/>
+      <c r="I25" s="207"/>
+      <c r="J25" s="208"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="38"/>
@@ -7076,8 +7085,8 @@
       <c r="F26" s="39"/>
       <c r="G26" s="39"/>
       <c r="H26" s="41"/>
-      <c r="I26" s="206"/>
-      <c r="J26" s="207"/>
+      <c r="I26" s="207"/>
+      <c r="J26" s="208"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1">
       <c r="A27" s="38"/>
@@ -7088,8 +7097,8 @@
       <c r="F27" s="39"/>
       <c r="G27" s="39"/>
       <c r="H27" s="41"/>
-      <c r="I27" s="206"/>
-      <c r="J27" s="207"/>
+      <c r="I27" s="207"/>
+      <c r="J27" s="208"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1">
       <c r="A28" s="38"/>
@@ -7100,8 +7109,8 @@
       <c r="F28" s="39"/>
       <c r="G28" s="39"/>
       <c r="H28" s="41"/>
-      <c r="I28" s="206"/>
-      <c r="J28" s="207"/>
+      <c r="I28" s="207"/>
+      <c r="J28" s="208"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1">
       <c r="A29" s="38"/>
@@ -7112,8 +7121,8 @@
       <c r="F29" s="39"/>
       <c r="G29" s="39"/>
       <c r="H29" s="41"/>
-      <c r="I29" s="206"/>
-      <c r="J29" s="207"/>
+      <c r="I29" s="207"/>
+      <c r="J29" s="208"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1">
       <c r="A30" s="38"/>
@@ -7124,8 +7133,8 @@
       <c r="F30" s="39"/>
       <c r="G30" s="39"/>
       <c r="H30" s="41"/>
-      <c r="I30" s="206"/>
-      <c r="J30" s="207"/>
+      <c r="I30" s="207"/>
+      <c r="J30" s="208"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1">
       <c r="A31" s="38"/>
@@ -7136,8 +7145,8 @@
       <c r="F31" s="39"/>
       <c r="G31" s="39"/>
       <c r="H31" s="41"/>
-      <c r="I31" s="206"/>
-      <c r="J31" s="207"/>
+      <c r="I31" s="207"/>
+      <c r="J31" s="208"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1">
       <c r="A32" s="38"/>
@@ -7148,8 +7157,8 @@
       <c r="F32" s="39"/>
       <c r="G32" s="39"/>
       <c r="H32" s="41"/>
-      <c r="I32" s="206"/>
-      <c r="J32" s="207"/>
+      <c r="I32" s="207"/>
+      <c r="J32" s="208"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="38"/>
@@ -7160,8 +7169,8 @@
       <c r="F33" s="39"/>
       <c r="G33" s="39"/>
       <c r="H33" s="41"/>
-      <c r="I33" s="206"/>
-      <c r="J33" s="207"/>
+      <c r="I33" s="207"/>
+      <c r="J33" s="208"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="38"/>
@@ -7172,8 +7181,8 @@
       <c r="F34" s="39"/>
       <c r="G34" s="39"/>
       <c r="H34" s="41"/>
-      <c r="I34" s="206"/>
-      <c r="J34" s="207"/>
+      <c r="I34" s="207"/>
+      <c r="J34" s="208"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1">
       <c r="A35" s="38"/>
@@ -7184,8 +7193,8 @@
       <c r="F35" s="39"/>
       <c r="G35" s="39"/>
       <c r="H35" s="41"/>
-      <c r="I35" s="206"/>
-      <c r="J35" s="207"/>
+      <c r="I35" s="207"/>
+      <c r="J35" s="208"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1">
       <c r="A36" s="38"/>
@@ -7196,8 +7205,8 @@
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
       <c r="H36" s="41"/>
-      <c r="I36" s="206"/>
-      <c r="J36" s="207"/>
+      <c r="I36" s="207"/>
+      <c r="J36" s="208"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="A37" s="38"/>
@@ -7208,8 +7217,8 @@
       <c r="F37" s="39"/>
       <c r="G37" s="39"/>
       <c r="H37" s="41"/>
-      <c r="I37" s="206"/>
-      <c r="J37" s="207"/>
+      <c r="I37" s="207"/>
+      <c r="J37" s="208"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1">
       <c r="A38" s="38"/>
@@ -7220,8 +7229,8 @@
       <c r="F38" s="39"/>
       <c r="G38" s="39"/>
       <c r="H38" s="41"/>
-      <c r="I38" s="206"/>
-      <c r="J38" s="207"/>
+      <c r="I38" s="207"/>
+      <c r="J38" s="208"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1">
       <c r="A39" s="38"/>
@@ -7232,8 +7241,8 @@
       <c r="F39" s="39"/>
       <c r="G39" s="39"/>
       <c r="H39" s="41"/>
-      <c r="I39" s="206"/>
-      <c r="J39" s="207"/>
+      <c r="I39" s="207"/>
+      <c r="J39" s="208"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1">
       <c r="A40" s="38"/>
@@ -7244,8 +7253,8 @@
       <c r="F40" s="39"/>
       <c r="G40" s="39"/>
       <c r="H40" s="41"/>
-      <c r="I40" s="206"/>
-      <c r="J40" s="207"/>
+      <c r="I40" s="207"/>
+      <c r="J40" s="208"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
       <c r="A41" s="38"/>
@@ -7256,8 +7265,8 @@
       <c r="F41" s="39"/>
       <c r="G41" s="39"/>
       <c r="H41" s="41"/>
-      <c r="I41" s="206"/>
-      <c r="J41" s="207"/>
+      <c r="I41" s="207"/>
+      <c r="J41" s="208"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1">
       <c r="A42" s="38"/>
@@ -7268,8 +7277,8 @@
       <c r="F42" s="39"/>
       <c r="G42" s="39"/>
       <c r="H42" s="41"/>
-      <c r="I42" s="206"/>
-      <c r="J42" s="207"/>
+      <c r="I42" s="207"/>
+      <c r="J42" s="208"/>
     </row>
     <row r="43" spans="1:10" ht="12" customHeight="1">
       <c r="A43" s="38"/>
@@ -7280,8 +7289,8 @@
       <c r="F43" s="39"/>
       <c r="G43" s="39"/>
       <c r="H43" s="41"/>
-      <c r="I43" s="206"/>
-      <c r="J43" s="207"/>
+      <c r="I43" s="207"/>
+      <c r="J43" s="208"/>
     </row>
     <row r="44" spans="1:10" ht="12" customHeight="1">
       <c r="A44" s="38"/>
@@ -7292,8 +7301,8 @@
       <c r="F44" s="39"/>
       <c r="G44" s="39"/>
       <c r="H44" s="41"/>
-      <c r="I44" s="206"/>
-      <c r="J44" s="207"/>
+      <c r="I44" s="207"/>
+      <c r="J44" s="208"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -7318,1193 +7327,1306 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="22" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="23" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="112" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="23" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="23" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" style="23" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.42578125" style="22" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="2" width="4.5703125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="23" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="112" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="23" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" style="23" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" style="23" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" style="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.42578125" style="22" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="196" t="s">
+    <row r="1" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A1" s="197" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="27" t="str">
+      <c r="G1" s="27" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="G1" s="214" t="s">
+      <c r="H1" s="215" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="215"/>
-      <c r="I1" s="216" t="str">
+      <c r="I1" s="216"/>
+      <c r="J1" s="217" t="str">
         <f>'Update History'!F1</f>
         <v>CRMF2080</v>
       </c>
-      <c r="J1" s="217"/>
       <c r="K1" s="218"/>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="219"/>
+      <c r="M1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="28" t="str">
+      <c r="N1" s="28" t="str">
         <f>'Update History'!H1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="O1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="57" t="str">
+      <c r="P1" s="57" t="str">
         <f>'Update History'!J1</f>
-        <v>Thị Phượng</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="29" t="s">
+        <v>Tấn Đạt</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A2" s="197"/>
+      <c r="B2" s="197"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="27" t="str">
+      <c r="G2" s="27" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT-CRM</v>
       </c>
-      <c r="G2" s="214" t="s">
+      <c r="H2" s="215" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="215"/>
-      <c r="I2" s="216" t="str">
+      <c r="I2" s="216"/>
+      <c r="J2" s="217" t="str">
         <f>'Update History'!F2</f>
         <v>Danh mục yêu cầu</v>
       </c>
-      <c r="J2" s="217"/>
       <c r="K2" s="218"/>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="219"/>
+      <c r="M2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="28" t="str">
+      <c r="N2" s="28" t="str">
         <f>'Update History'!H2</f>
         <v>25/03/2017</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="O2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="57" t="str">
+      <c r="P2" s="57" t="str">
         <f>'Update History'!J2</f>
-        <v>25/03/2017</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="21" customFormat="1" ht="23.25" customHeight="1">
+        <v>26/01/2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="21" customFormat="1" ht="23.25" customHeight="1">
       <c r="A4" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="D4" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="E4" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="F4" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="G4" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="111" t="s">
+      <c r="H4" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="I4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="J4" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="K4" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="L4" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="M4" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="N4" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="O4" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="P4" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="25" customFormat="1" ht="11.25" customHeight="1">
+    <row r="5" spans="1:16" s="25" customFormat="1" ht="11.25" customHeight="1">
       <c r="A5" s="107">
-        <v>2</v>
-      </c>
-      <c r="B5" s="107" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="107">
+      <c r="D5" s="107">
         <v>0</v>
       </c>
-      <c r="D5" s="119" t="s">
+      <c r="E5" s="119" t="s">
         <v>249</v>
       </c>
-      <c r="E5" s="108"/>
       <c r="F5" s="108"/>
-      <c r="G5" s="108" t="s">
+      <c r="G5" s="108"/>
+      <c r="H5" s="108" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="109"/>
-      <c r="I5" s="110"/>
+      <c r="I5" s="109"/>
       <c r="J5" s="110"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="108"/>
+      <c r="K5" s="110"/>
+      <c r="L5" s="109"/>
       <c r="M5" s="108"/>
       <c r="N5" s="108"/>
       <c r="O5" s="108"/>
-    </row>
-    <row r="6" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="P5" s="108"/>
+    </row>
+    <row r="6" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A6" s="107">
-        <v>4</v>
-      </c>
-      <c r="B6" s="107" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="107">
+      <c r="D6" s="107">
         <v>1</v>
       </c>
-      <c r="D6" s="119" t="s">
+      <c r="E6" s="119" t="s">
         <v>250</v>
       </c>
-      <c r="E6" s="108"/>
       <c r="F6" s="108"/>
-      <c r="G6" s="108" t="s">
+      <c r="G6" s="108"/>
+      <c r="H6" s="108" t="s">
         <v>180</v>
       </c>
-      <c r="H6" s="109"/>
-      <c r="I6" s="110"/>
+      <c r="I6" s="109"/>
       <c r="J6" s="110"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="108"/>
+      <c r="K6" s="110"/>
+      <c r="L6" s="109"/>
       <c r="M6" s="108"/>
       <c r="N6" s="108"/>
       <c r="O6" s="108"/>
-    </row>
-    <row r="7" spans="1:15" s="25" customFormat="1" ht="48.75" customHeight="1">
+      <c r="P6" s="108"/>
+    </row>
+    <row r="7" spans="1:16" s="25" customFormat="1" ht="48.75" customHeight="1">
       <c r="A7" s="107">
-        <v>5</v>
-      </c>
-      <c r="B7" s="107" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="107">
+      <c r="D7" s="107">
         <v>2</v>
       </c>
-      <c r="D7" s="119" t="s">
+      <c r="E7" s="119" t="s">
         <v>161</v>
-      </c>
-      <c r="E7" s="108" t="s">
-        <v>170</v>
       </c>
       <c r="F7" s="108" t="s">
         <v>170</v>
       </c>
       <c r="G7" s="108" t="s">
+        <v>170</v>
+      </c>
+      <c r="H7" s="108" t="s">
         <v>181</v>
       </c>
-      <c r="H7" s="109" t="s">
+      <c r="I7" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="I7" s="110"/>
       <c r="J7" s="110"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="108"/>
+      <c r="K7" s="110"/>
+      <c r="L7" s="109"/>
       <c r="M7" s="108"/>
       <c r="N7" s="108"/>
-      <c r="O7" s="122" t="s">
+      <c r="O7" s="108"/>
+      <c r="P7" s="122" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+    <row r="8" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="107">
-        <v>6</v>
-      </c>
-      <c r="B8" s="107" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="107">
+      <c r="D8" s="107">
         <v>3</v>
       </c>
-      <c r="D8" s="119" t="s">
+      <c r="E8" s="119" t="s">
         <v>254</v>
-      </c>
-      <c r="E8" s="108" t="s">
-        <v>295</v>
       </c>
       <c r="F8" s="108" t="s">
         <v>295</v>
       </c>
       <c r="G8" s="108" t="s">
+        <v>295</v>
+      </c>
+      <c r="H8" s="108" t="s">
         <v>156</v>
       </c>
-      <c r="H8" s="109" t="s">
+      <c r="I8" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="I8" s="110">
+      <c r="J8" s="110">
         <v>50</v>
       </c>
-      <c r="J8" s="110"/>
-      <c r="K8" s="109" t="s">
+      <c r="K8" s="110"/>
+      <c r="L8" s="109" t="s">
         <v>182</v>
       </c>
-      <c r="L8" s="108"/>
       <c r="M8" s="108"/>
       <c r="N8" s="108"/>
       <c r="O8" s="108"/>
-    </row>
-    <row r="9" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="P8" s="108"/>
+    </row>
+    <row r="9" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A9" s="107">
-        <v>7</v>
-      </c>
-      <c r="B9" s="107" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="107"/>
+      <c r="C9" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="107">
+      <c r="D9" s="107">
         <v>4</v>
       </c>
-      <c r="D9" s="119" t="s">
+      <c r="E9" s="119" t="s">
         <v>255</v>
-      </c>
-      <c r="E9" s="108" t="s">
-        <v>256</v>
       </c>
       <c r="F9" s="108" t="s">
         <v>256</v>
       </c>
       <c r="G9" s="108" t="s">
+        <v>256</v>
+      </c>
+      <c r="H9" s="108" t="s">
         <v>156</v>
       </c>
-      <c r="H9" s="109" t="s">
+      <c r="I9" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="I9" s="110">
+      <c r="J9" s="110">
         <v>250</v>
       </c>
-      <c r="J9" s="110"/>
-      <c r="K9" s="109" t="s">
+      <c r="K9" s="110"/>
+      <c r="L9" s="109" t="s">
         <v>182</v>
       </c>
-      <c r="L9" s="108"/>
       <c r="M9" s="108"/>
       <c r="N9" s="108"/>
       <c r="O9" s="108"/>
-    </row>
-    <row r="10" spans="1:15" s="25" customFormat="1" ht="45">
+      <c r="P9" s="108"/>
+    </row>
+    <row r="10" spans="1:16" s="25" customFormat="1" ht="45">
       <c r="A10" s="107">
-        <v>12</v>
-      </c>
-      <c r="B10" s="107" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="107"/>
+      <c r="C10" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C10" s="107">
+      <c r="D10" s="107">
         <v>5</v>
       </c>
-      <c r="D10" s="140" t="s">
+      <c r="E10" s="140" t="s">
         <v>257</v>
-      </c>
-      <c r="E10" s="108" t="s">
-        <v>252</v>
       </c>
       <c r="F10" s="108" t="s">
         <v>252</v>
       </c>
       <c r="G10" s="108" t="s">
+        <v>252</v>
+      </c>
+      <c r="H10" s="108" t="s">
         <v>177</v>
       </c>
-      <c r="H10" s="109" t="s">
+      <c r="I10" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="I10" s="110">
-        <v>25</v>
-      </c>
       <c r="J10" s="110"/>
-      <c r="K10" s="109" t="s">
+      <c r="K10" s="110"/>
+      <c r="L10" s="109" t="s">
         <v>182</v>
       </c>
-      <c r="L10" s="108"/>
       <c r="M10" s="108"/>
       <c r="N10" s="108"/>
-      <c r="O10" s="122" t="s">
+      <c r="O10" s="108"/>
+      <c r="P10" s="122" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+    <row r="11" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="107">
-        <v>8</v>
-      </c>
-      <c r="B11" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="107"/>
+      <c r="C11" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="107">
+      <c r="D11" s="107">
         <v>6</v>
       </c>
-      <c r="D11" s="119" t="s">
+      <c r="E11" s="119" t="s">
         <v>233</v>
-      </c>
-      <c r="E11" s="108" t="s">
-        <v>234</v>
       </c>
       <c r="F11" s="108" t="s">
         <v>234</v>
       </c>
       <c r="G11" s="108" t="s">
+        <v>234</v>
+      </c>
+      <c r="H11" s="108" t="s">
         <v>156</v>
       </c>
-      <c r="H11" s="109" t="s">
+      <c r="I11" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="I11" s="110">
+      <c r="J11" s="110">
         <v>100</v>
       </c>
-      <c r="J11" s="110"/>
-      <c r="K11" s="109" t="s">
+      <c r="K11" s="110"/>
+      <c r="L11" s="109" t="s">
         <v>182</v>
       </c>
-      <c r="L11" s="108"/>
       <c r="M11" s="108"/>
       <c r="N11" s="108"/>
       <c r="O11" s="108"/>
-    </row>
-    <row r="12" spans="1:15" s="25" customFormat="1" ht="45">
+      <c r="P11" s="108"/>
+    </row>
+    <row r="12" spans="1:16" s="25" customFormat="1" ht="45">
       <c r="A12" s="107">
-        <v>9</v>
-      </c>
-      <c r="B12" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="107"/>
+      <c r="C12" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C12" s="107">
+      <c r="D12" s="107">
         <v>7</v>
       </c>
-      <c r="D12" s="140" t="s">
+      <c r="E12" s="140" t="s">
         <v>258</v>
-      </c>
-      <c r="E12" s="108" t="s">
-        <v>259</v>
       </c>
       <c r="F12" s="108" t="s">
         <v>259</v>
       </c>
       <c r="G12" s="108" t="s">
+        <v>259</v>
+      </c>
+      <c r="H12" s="108" t="s">
         <v>177</v>
       </c>
-      <c r="H12" s="109" t="s">
+      <c r="I12" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="I12" s="110">
-        <v>25</v>
-      </c>
       <c r="J12" s="110"/>
-      <c r="K12" s="109" t="s">
+      <c r="K12" s="110"/>
+      <c r="L12" s="109" t="s">
         <v>182</v>
       </c>
-      <c r="L12" s="108"/>
       <c r="M12" s="108"/>
       <c r="N12" s="108"/>
-      <c r="O12" s="122" t="s">
+      <c r="O12" s="108"/>
+      <c r="P12" s="122" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A13" s="107">
-        <v>19</v>
-      </c>
-      <c r="B13" s="107" t="s">
+    <row r="13" spans="1:16" s="162" customFormat="1" ht="45">
+      <c r="A13" s="155">
+        <v>9</v>
+      </c>
+      <c r="B13" s="155">
+        <v>92</v>
+      </c>
+      <c r="C13" s="155" t="s">
+        <v>323</v>
+      </c>
+      <c r="D13" s="155">
+        <v>8</v>
+      </c>
+      <c r="E13" s="156" t="s">
+        <v>320</v>
+      </c>
+      <c r="F13" s="158" t="s">
+        <v>321</v>
+      </c>
+      <c r="G13" s="158" t="s">
+        <v>321</v>
+      </c>
+      <c r="H13" s="158" t="s">
+        <v>177</v>
+      </c>
+      <c r="I13" s="159" t="s">
+        <v>157</v>
+      </c>
+      <c r="J13" s="160"/>
+      <c r="K13" s="160"/>
+      <c r="L13" s="159" t="s">
+        <v>182</v>
+      </c>
+      <c r="M13" s="158"/>
+      <c r="N13" s="158"/>
+      <c r="O13" s="158"/>
+      <c r="P13" s="161" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="162" customFormat="1" ht="45">
+      <c r="A14" s="155">
+        <v>10</v>
+      </c>
+      <c r="B14" s="155">
+        <v>92</v>
+      </c>
+      <c r="C14" s="155" t="s">
+        <v>323</v>
+      </c>
+      <c r="D14" s="155">
+        <v>9</v>
+      </c>
+      <c r="E14" s="156" t="s">
+        <v>324</v>
+      </c>
+      <c r="F14" s="158" t="s">
+        <v>325</v>
+      </c>
+      <c r="G14" s="158" t="s">
+        <v>325</v>
+      </c>
+      <c r="H14" s="158" t="s">
+        <v>177</v>
+      </c>
+      <c r="I14" s="159" t="s">
+        <v>157</v>
+      </c>
+      <c r="J14" s="160"/>
+      <c r="K14" s="160"/>
+      <c r="L14" s="159" t="s">
+        <v>182</v>
+      </c>
+      <c r="M14" s="158"/>
+      <c r="N14" s="158"/>
+      <c r="O14" s="158"/>
+      <c r="P14" s="161" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A15" s="107">
+        <v>11</v>
+      </c>
+      <c r="B15" s="107"/>
+      <c r="C15" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="107">
-        <v>8</v>
-      </c>
-      <c r="D13" s="125" t="s">
+      <c r="D15" s="107">
+        <v>10</v>
+      </c>
+      <c r="E15" s="125" t="s">
         <v>164</v>
       </c>
-      <c r="E13" s="108" t="s">
+      <c r="F15" s="108" t="s">
         <v>173</v>
       </c>
-      <c r="F13" s="108"/>
-      <c r="G13" s="108" t="s">
+      <c r="G15" s="108"/>
+      <c r="H15" s="108" t="s">
         <v>159</v>
       </c>
-      <c r="H13" s="109"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="109"/>
-      <c r="L13" s="108"/>
-      <c r="M13" s="108"/>
-      <c r="N13" s="108"/>
-      <c r="O13" s="108"/>
-    </row>
-    <row r="14" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A14" s="107">
-        <v>20</v>
-      </c>
-      <c r="B14" s="107" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="107">
-        <v>9</v>
-      </c>
-      <c r="D14" s="125" t="s">
-        <v>165</v>
-      </c>
-      <c r="E14" s="108" t="s">
-        <v>174</v>
-      </c>
-      <c r="F14" s="108"/>
-      <c r="G14" s="108" t="s">
-        <v>159</v>
-      </c>
-      <c r="H14" s="109"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="109"/>
-      <c r="L14" s="108"/>
-      <c r="M14" s="108"/>
-      <c r="N14" s="108"/>
-      <c r="O14" s="123" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A15" s="107">
-        <v>19</v>
-      </c>
-      <c r="B15" s="107" t="s">
-        <v>155</v>
-      </c>
-      <c r="C15" s="107">
-        <v>10</v>
-      </c>
-      <c r="D15" s="125" t="s">
-        <v>209</v>
-      </c>
-      <c r="E15" s="108" t="s">
-        <v>213</v>
-      </c>
-      <c r="F15" s="108"/>
-      <c r="G15" s="108" t="s">
-        <v>159</v>
-      </c>
-      <c r="H15" s="109"/>
-      <c r="I15" s="110"/>
+      <c r="I15" s="109"/>
       <c r="J15" s="110"/>
-      <c r="K15" s="109"/>
-      <c r="L15" s="108"/>
+      <c r="K15" s="110"/>
+      <c r="L15" s="109"/>
       <c r="M15" s="108"/>
       <c r="N15" s="108"/>
       <c r="O15" s="108"/>
-    </row>
-    <row r="16" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="P15" s="108"/>
+    </row>
+    <row r="16" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A16" s="107">
-        <v>36</v>
-      </c>
-      <c r="B16" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="107"/>
+      <c r="C16" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="107">
+      <c r="D16" s="107">
         <v>11</v>
       </c>
-      <c r="D16" s="120" t="s">
+      <c r="E16" s="125" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16" s="108" t="s">
+        <v>174</v>
+      </c>
+      <c r="G16" s="108"/>
+      <c r="H16" s="108" t="s">
+        <v>159</v>
+      </c>
+      <c r="I16" s="109"/>
+      <c r="J16" s="110"/>
+      <c r="K16" s="110"/>
+      <c r="L16" s="109"/>
+      <c r="M16" s="108"/>
+      <c r="N16" s="108"/>
+      <c r="O16" s="108"/>
+      <c r="P16" s="123" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A17" s="107">
+        <v>13</v>
+      </c>
+      <c r="B17" s="107"/>
+      <c r="C17" s="107" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="107">
+        <v>12</v>
+      </c>
+      <c r="E17" s="125" t="s">
+        <v>209</v>
+      </c>
+      <c r="F17" s="108" t="s">
+        <v>213</v>
+      </c>
+      <c r="G17" s="108"/>
+      <c r="H17" s="108" t="s">
+        <v>159</v>
+      </c>
+      <c r="I17" s="109"/>
+      <c r="J17" s="110"/>
+      <c r="K17" s="110"/>
+      <c r="L17" s="109"/>
+      <c r="M17" s="108"/>
+      <c r="N17" s="108"/>
+      <c r="O17" s="108"/>
+      <c r="P17" s="108"/>
+    </row>
+    <row r="18" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A18" s="107">
+        <v>14</v>
+      </c>
+      <c r="B18" s="107"/>
+      <c r="C18" s="107" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="107">
+        <v>13</v>
+      </c>
+      <c r="E18" s="120" t="s">
         <v>238</v>
       </c>
-      <c r="E16" s="121" t="s">
+      <c r="F18" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="F16" s="121"/>
-      <c r="G16" s="120" t="s">
+      <c r="G18" s="121"/>
+      <c r="H18" s="120" t="s">
         <v>159</v>
       </c>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107"/>
-      <c r="J16" s="107"/>
-      <c r="K16" s="107"/>
-      <c r="L16" s="107"/>
-      <c r="M16" s="107"/>
-      <c r="N16" s="107"/>
-      <c r="O16" s="123" t="s">
+      <c r="I18" s="107"/>
+      <c r="J18" s="107"/>
+      <c r="K18" s="107"/>
+      <c r="L18" s="107"/>
+      <c r="M18" s="107"/>
+      <c r="N18" s="107"/>
+      <c r="O18" s="107"/>
+      <c r="P18" s="123" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A17" s="107">
-        <v>37</v>
-      </c>
-      <c r="B17" s="107" t="s">
+    <row r="19" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A19" s="107">
+        <v>15</v>
+      </c>
+      <c r="B19" s="107"/>
+      <c r="C19" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C17" s="107">
-        <v>12</v>
-      </c>
-      <c r="D17" s="120" t="s">
+      <c r="D19" s="107">
+        <v>14</v>
+      </c>
+      <c r="E19" s="120" t="s">
         <v>184</v>
       </c>
-      <c r="E17" s="121" t="s">
+      <c r="F19" s="121" t="s">
         <v>185</v>
       </c>
-      <c r="F17" s="121"/>
-      <c r="G17" s="120" t="s">
+      <c r="G19" s="121"/>
+      <c r="H19" s="120" t="s">
         <v>159</v>
       </c>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107"/>
-      <c r="J17" s="107"/>
-      <c r="K17" s="107"/>
-      <c r="L17" s="107"/>
-      <c r="M17" s="107"/>
-      <c r="N17" s="107"/>
-      <c r="O17" s="123" t="s">
+      <c r="I19" s="107"/>
+      <c r="J19" s="107"/>
+      <c r="K19" s="107"/>
+      <c r="L19" s="107"/>
+      <c r="M19" s="107"/>
+      <c r="N19" s="107"/>
+      <c r="O19" s="107"/>
+      <c r="P19" s="123" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A18" s="107">
-        <v>20</v>
-      </c>
-      <c r="B18" s="107" t="s">
+    <row r="20" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A20" s="107">
+        <v>16</v>
+      </c>
+      <c r="B20" s="107"/>
+      <c r="C20" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C18" s="107">
-        <v>13</v>
-      </c>
-      <c r="D18" s="125" t="s">
+      <c r="D20" s="107">
+        <v>15</v>
+      </c>
+      <c r="E20" s="125" t="s">
         <v>210</v>
       </c>
-      <c r="E18" s="108" t="s">
+      <c r="F20" s="108" t="s">
         <v>214</v>
       </c>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108" t="s">
+      <c r="G20" s="108"/>
+      <c r="H20" s="108" t="s">
         <v>159</v>
       </c>
-      <c r="H18" s="109"/>
-      <c r="I18" s="110"/>
-      <c r="J18" s="110"/>
-      <c r="K18" s="109"/>
-      <c r="L18" s="108"/>
-      <c r="M18" s="108"/>
-      <c r="N18" s="108"/>
-      <c r="O18" s="123"/>
-    </row>
-    <row r="19" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A19" s="107">
-        <v>20</v>
-      </c>
-      <c r="B19" s="107" t="s">
-        <v>155</v>
-      </c>
-      <c r="C19" s="107">
-        <v>14</v>
-      </c>
-      <c r="D19" s="119" t="s">
-        <v>211</v>
-      </c>
-      <c r="E19" s="108" t="s">
-        <v>215</v>
-      </c>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108" t="s">
-        <v>159</v>
-      </c>
-      <c r="H19" s="109"/>
-      <c r="I19" s="110"/>
-      <c r="J19" s="110"/>
-      <c r="K19" s="109"/>
-      <c r="L19" s="108"/>
-      <c r="M19" s="108"/>
-      <c r="N19" s="108"/>
-      <c r="O19" s="123"/>
-    </row>
-    <row r="20" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A20" s="107">
-        <v>17</v>
-      </c>
-      <c r="B20" s="107" t="s">
-        <v>155</v>
-      </c>
-      <c r="C20" s="107">
-        <v>15</v>
-      </c>
-      <c r="D20" s="119" t="s">
-        <v>162</v>
-      </c>
-      <c r="E20" s="108" t="s">
-        <v>171</v>
-      </c>
-      <c r="F20" s="108"/>
-      <c r="G20" s="108" t="s">
-        <v>159</v>
-      </c>
-      <c r="H20" s="109"/>
-      <c r="I20" s="110"/>
+      <c r="I20" s="109"/>
       <c r="J20" s="110"/>
-      <c r="K20" s="109"/>
-      <c r="L20" s="108"/>
+      <c r="K20" s="110"/>
+      <c r="L20" s="109"/>
       <c r="M20" s="108"/>
       <c r="N20" s="108"/>
       <c r="O20" s="108"/>
-    </row>
-    <row r="21" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="P20" s="123"/>
+    </row>
+    <row r="21" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="107">
-        <v>18</v>
-      </c>
-      <c r="B21" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="107"/>
+      <c r="C21" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C21" s="107">
+      <c r="D21" s="107">
         <v>16</v>
       </c>
-      <c r="D21" s="119" t="s">
-        <v>163</v>
-      </c>
-      <c r="E21" s="108" t="s">
-        <v>172</v>
-      </c>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108" t="s">
+      <c r="E21" s="119" t="s">
+        <v>211</v>
+      </c>
+      <c r="F21" s="108" t="s">
+        <v>215</v>
+      </c>
+      <c r="G21" s="108"/>
+      <c r="H21" s="108" t="s">
         <v>159</v>
       </c>
-      <c r="H21" s="109"/>
-      <c r="I21" s="110"/>
+      <c r="I21" s="109"/>
       <c r="J21" s="110"/>
-      <c r="K21" s="109"/>
-      <c r="L21" s="108"/>
+      <c r="K21" s="110"/>
+      <c r="L21" s="109"/>
       <c r="M21" s="108"/>
       <c r="N21" s="108"/>
       <c r="O21" s="108"/>
-    </row>
-    <row r="22" spans="1:15" s="25" customFormat="1" ht="45">
+      <c r="P21" s="123"/>
+    </row>
+    <row r="22" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A22" s="107">
-        <v>34</v>
-      </c>
-      <c r="B22" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="107"/>
+      <c r="C22" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C22" s="107">
+      <c r="D22" s="107">
         <v>17</v>
       </c>
-      <c r="D22" s="140" t="s">
+      <c r="E22" s="119" t="s">
+        <v>162</v>
+      </c>
+      <c r="F22" s="108" t="s">
+        <v>171</v>
+      </c>
+      <c r="G22" s="108"/>
+      <c r="H22" s="108" t="s">
+        <v>159</v>
+      </c>
+      <c r="I22" s="109"/>
+      <c r="J22" s="110"/>
+      <c r="K22" s="110"/>
+      <c r="L22" s="109"/>
+      <c r="M22" s="108"/>
+      <c r="N22" s="108"/>
+      <c r="O22" s="108"/>
+      <c r="P22" s="108"/>
+    </row>
+    <row r="23" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A23" s="107">
+        <v>19</v>
+      </c>
+      <c r="B23" s="107"/>
+      <c r="C23" s="107" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="107">
+        <v>18</v>
+      </c>
+      <c r="E23" s="119" t="s">
+        <v>163</v>
+      </c>
+      <c r="F23" s="108" t="s">
+        <v>172</v>
+      </c>
+      <c r="G23" s="108"/>
+      <c r="H23" s="108" t="s">
+        <v>159</v>
+      </c>
+      <c r="I23" s="109"/>
+      <c r="J23" s="110"/>
+      <c r="K23" s="110"/>
+      <c r="L23" s="109"/>
+      <c r="M23" s="108"/>
+      <c r="N23" s="108"/>
+      <c r="O23" s="108"/>
+      <c r="P23" s="108"/>
+    </row>
+    <row r="24" spans="1:16" s="25" customFormat="1" ht="45">
+      <c r="A24" s="107">
+        <v>20</v>
+      </c>
+      <c r="B24" s="107"/>
+      <c r="C24" s="107" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="107">
+        <v>19</v>
+      </c>
+      <c r="E24" s="140" t="s">
         <v>166</v>
       </c>
-      <c r="E22" s="120" t="s">
+      <c r="F24" s="120" t="s">
         <v>188</v>
       </c>
-      <c r="F22" s="108"/>
-      <c r="G22" s="108" t="s">
+      <c r="G24" s="108"/>
+      <c r="H24" s="108" t="s">
         <v>177</v>
       </c>
-      <c r="H22" s="109" t="s">
+      <c r="I24" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="I22" s="110"/>
-      <c r="J22" s="110"/>
-      <c r="K22" s="109" t="s">
+      <c r="J24" s="110"/>
+      <c r="K24" s="110"/>
+      <c r="L24" s="109" t="s">
         <v>160</v>
       </c>
-      <c r="L22" s="108"/>
-      <c r="M22" s="108"/>
-      <c r="N22" s="109">
-        <v>25</v>
-      </c>
-      <c r="O22" s="122" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A23" s="107">
-        <v>35</v>
-      </c>
-      <c r="B23" s="107" t="s">
-        <v>155</v>
-      </c>
-      <c r="C23" s="107">
-        <v>18</v>
-      </c>
-      <c r="D23" s="140" t="s">
-        <v>167</v>
-      </c>
-      <c r="E23" s="120" t="s">
-        <v>189</v>
-      </c>
-      <c r="F23" s="108"/>
-      <c r="G23" s="108" t="s">
-        <v>178</v>
-      </c>
-      <c r="H23" s="109" t="s">
-        <v>158</v>
-      </c>
-      <c r="I23" s="110"/>
-      <c r="J23" s="110"/>
-      <c r="K23" s="109" t="s">
-        <v>160</v>
-      </c>
-      <c r="L23" s="108"/>
-      <c r="M23" s="108"/>
-      <c r="N23" s="109">
-        <v>1</v>
-      </c>
-      <c r="O23" s="108"/>
-    </row>
-    <row r="24" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A24" s="107">
-        <v>21</v>
-      </c>
-      <c r="B24" s="107" t="s">
-        <v>155</v>
-      </c>
-      <c r="C24" s="107">
-        <v>19</v>
-      </c>
-      <c r="D24" s="119" t="s">
-        <v>168</v>
-      </c>
-      <c r="E24" s="108" t="s">
-        <v>175</v>
-      </c>
-      <c r="F24" s="108"/>
-      <c r="G24" s="108" t="s">
-        <v>176</v>
-      </c>
-      <c r="H24" s="109"/>
-      <c r="I24" s="110"/>
-      <c r="J24" s="110"/>
-      <c r="K24" s="109"/>
-      <c r="L24" s="108"/>
       <c r="M24" s="108"/>
       <c r="N24" s="108"/>
-      <c r="O24" s="108"/>
-    </row>
-    <row r="25" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="O24" s="109">
+        <v>25</v>
+      </c>
+      <c r="P24" s="122" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A25" s="107">
+        <v>21</v>
+      </c>
+      <c r="B25" s="107"/>
+      <c r="C25" s="107" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="107">
+        <v>20</v>
+      </c>
+      <c r="E25" s="140" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25" s="120" t="s">
+        <v>189</v>
+      </c>
+      <c r="G25" s="108"/>
+      <c r="H25" s="108" t="s">
+        <v>178</v>
+      </c>
+      <c r="I25" s="109" t="s">
+        <v>158</v>
+      </c>
+      <c r="J25" s="110"/>
+      <c r="K25" s="110"/>
+      <c r="L25" s="109" t="s">
+        <v>160</v>
+      </c>
+      <c r="M25" s="108"/>
+      <c r="N25" s="108"/>
+      <c r="O25" s="109">
+        <v>1</v>
+      </c>
+      <c r="P25" s="108"/>
+    </row>
+    <row r="26" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A26" s="107">
         <v>22</v>
       </c>
-      <c r="B25" s="107" t="s">
+      <c r="B26" s="107"/>
+      <c r="C26" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C25" s="127">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="D25" s="119" t="s">
-        <v>169</v>
-      </c>
-      <c r="E25" s="108" t="s">
-        <v>191</v>
-      </c>
-      <c r="F25" s="108"/>
-      <c r="G25" s="108" t="s">
+      <c r="D26" s="107">
+        <v>21</v>
+      </c>
+      <c r="E26" s="119" t="s">
+        <v>168</v>
+      </c>
+      <c r="F26" s="108" t="s">
+        <v>175</v>
+      </c>
+      <c r="G26" s="108"/>
+      <c r="H26" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="H25" s="109"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="110"/>
-      <c r="K25" s="109"/>
-      <c r="L25" s="108"/>
-      <c r="M25" s="108"/>
-      <c r="N25" s="124">
-        <v>0</v>
-      </c>
-      <c r="O25" s="121" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A26" s="107">
-        <v>23</v>
-      </c>
-      <c r="B26" s="107" t="s">
-        <v>155</v>
-      </c>
-      <c r="C26" s="127">
-        <v>19.2</v>
-      </c>
-      <c r="D26" s="125" t="s">
-        <v>212</v>
-      </c>
-      <c r="E26" s="108" t="s">
-        <v>216</v>
-      </c>
-      <c r="F26" s="108" t="s">
-        <v>216</v>
-      </c>
-      <c r="G26" s="108" t="s">
-        <v>176</v>
-      </c>
-      <c r="H26" s="109" t="s">
-        <v>157</v>
-      </c>
-      <c r="I26" s="110"/>
+      <c r="I26" s="109"/>
       <c r="J26" s="110"/>
-      <c r="K26" s="109" t="s">
-        <v>160</v>
-      </c>
-      <c r="L26" s="108"/>
+      <c r="K26" s="110"/>
+      <c r="L26" s="109"/>
       <c r="M26" s="108"/>
       <c r="N26" s="108"/>
       <c r="O26" s="108"/>
-    </row>
-    <row r="27" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="P26" s="108"/>
+    </row>
+    <row r="27" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A27" s="107">
         <v>23</v>
       </c>
-      <c r="B27" s="107" t="s">
+      <c r="B27" s="107"/>
+      <c r="C27" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C27" s="127">
-        <v>19.3</v>
-      </c>
-      <c r="D27" s="119" t="s">
-        <v>161</v>
-      </c>
-      <c r="E27" s="108" t="s">
-        <v>170</v>
+      <c r="D27" s="127">
+        <v>21.1</v>
+      </c>
+      <c r="E27" s="119" t="s">
+        <v>169</v>
       </c>
       <c r="F27" s="108" t="s">
-        <v>170</v>
-      </c>
-      <c r="G27" s="108" t="s">
+        <v>191</v>
+      </c>
+      <c r="G27" s="108"/>
+      <c r="H27" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="H27" s="109" t="s">
-        <v>157</v>
-      </c>
-      <c r="I27" s="110"/>
+      <c r="I27" s="109"/>
       <c r="J27" s="110"/>
-      <c r="K27" s="109" t="s">
-        <v>160</v>
-      </c>
-      <c r="L27" s="108"/>
+      <c r="K27" s="110"/>
+      <c r="L27" s="109"/>
       <c r="M27" s="108"/>
       <c r="N27" s="108"/>
-      <c r="O27" s="108"/>
-    </row>
-    <row r="28" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="O27" s="124">
+        <v>0</v>
+      </c>
+      <c r="P27" s="121" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A28" s="107">
         <v>24</v>
       </c>
-      <c r="B28" s="107" t="s">
+      <c r="B28" s="107"/>
+      <c r="C28" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="127">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="D28" s="119" t="s">
-        <v>255</v>
-      </c>
-      <c r="E28" s="108" t="s">
-        <v>256</v>
+      <c r="D28" s="127">
+        <v>21.2</v>
+      </c>
+      <c r="E28" s="125" t="s">
+        <v>212</v>
       </c>
       <c r="F28" s="108" t="s">
-        <v>256</v>
+        <v>216</v>
       </c>
       <c r="G28" s="108" t="s">
+        <v>216</v>
+      </c>
+      <c r="H28" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="H28" s="109" t="s">
+      <c r="I28" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="I28" s="110"/>
       <c r="J28" s="110"/>
-      <c r="K28" s="109" t="s">
+      <c r="K28" s="110"/>
+      <c r="L28" s="109" t="s">
         <v>160</v>
       </c>
-      <c r="L28" s="108"/>
       <c r="M28" s="108"/>
       <c r="N28" s="108"/>
       <c r="O28" s="108"/>
-    </row>
-    <row r="29" spans="1:15" s="25" customFormat="1" ht="11.25">
+      <c r="P28" s="108"/>
+    </row>
+    <row r="29" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A29" s="107">
         <v>25</v>
       </c>
-      <c r="B29" s="107" t="s">
+      <c r="B29" s="107"/>
+      <c r="C29" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C29" s="127">
-        <v>19.5</v>
-      </c>
-      <c r="D29" s="119" t="s">
-        <v>254</v>
-      </c>
-      <c r="E29" s="108" t="s">
-        <v>261</v>
+      <c r="D29" s="127">
+        <v>21.3</v>
+      </c>
+      <c r="E29" s="119" t="s">
+        <v>161</v>
       </c>
       <c r="F29" s="108" t="s">
-        <v>261</v>
+        <v>170</v>
       </c>
       <c r="G29" s="108" t="s">
+        <v>170</v>
+      </c>
+      <c r="H29" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="H29" s="109" t="s">
+      <c r="I29" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="I29" s="110"/>
       <c r="J29" s="110"/>
-      <c r="K29" s="109" t="s">
+      <c r="K29" s="110"/>
+      <c r="L29" s="109" t="s">
         <v>160</v>
       </c>
-      <c r="L29" s="108"/>
       <c r="M29" s="108"/>
       <c r="N29" s="108"/>
       <c r="O29" s="108"/>
-    </row>
-    <row r="30" spans="1:15" s="25" customFormat="1" ht="11.25">
+      <c r="P29" s="108"/>
+    </row>
+    <row r="30" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A30" s="107">
-        <v>25</v>
-      </c>
-      <c r="B30" s="107" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="107"/>
+      <c r="C30" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C30" s="127">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="D30" s="141" t="s">
-        <v>296</v>
-      </c>
-      <c r="E30" s="108" t="s">
-        <v>297</v>
+      <c r="D30" s="127">
+        <v>21.4</v>
+      </c>
+      <c r="E30" s="119" t="s">
+        <v>255</v>
       </c>
       <c r="F30" s="108" t="s">
-        <v>297</v>
+        <v>256</v>
       </c>
       <c r="G30" s="108" t="s">
+        <v>256</v>
+      </c>
+      <c r="H30" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="H30" s="109" t="s">
+      <c r="I30" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="I30" s="110"/>
       <c r="J30" s="110"/>
-      <c r="K30" s="109" t="s">
+      <c r="K30" s="110"/>
+      <c r="L30" s="109" t="s">
         <v>160</v>
       </c>
-      <c r="L30" s="108"/>
       <c r="M30" s="108"/>
       <c r="N30" s="108"/>
       <c r="O30" s="108"/>
-    </row>
-    <row r="31" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="P30" s="108"/>
+    </row>
+    <row r="31" spans="1:16" s="25" customFormat="1" ht="11.25">
       <c r="A31" s="107">
-        <v>26</v>
-      </c>
-      <c r="B31" s="107" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="107"/>
+      <c r="C31" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C31" s="127">
-        <v>19.7</v>
-      </c>
-      <c r="D31" s="135" t="s">
-        <v>233</v>
-      </c>
-      <c r="E31" s="108" t="s">
-        <v>262</v>
+      <c r="D31" s="127">
+        <v>21.5</v>
+      </c>
+      <c r="E31" s="119" t="s">
+        <v>254</v>
       </c>
       <c r="F31" s="108" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G31" s="108" t="s">
+        <v>261</v>
+      </c>
+      <c r="H31" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="H31" s="109" t="s">
+      <c r="I31" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="I31" s="110"/>
       <c r="J31" s="110"/>
-      <c r="K31" s="109" t="s">
+      <c r="K31" s="110"/>
+      <c r="L31" s="109" t="s">
         <v>160</v>
       </c>
-      <c r="L31" s="108"/>
       <c r="M31" s="108"/>
       <c r="N31" s="108"/>
       <c r="O31" s="108"/>
-    </row>
-    <row r="32" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="P31" s="108"/>
+    </row>
+    <row r="32" spans="1:16" s="25" customFormat="1" ht="11.25">
       <c r="A32" s="107">
-        <v>27</v>
-      </c>
-      <c r="B32" s="107" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="107"/>
+      <c r="C32" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C32" s="127">
-        <v>19.8</v>
-      </c>
-      <c r="D32" s="135" t="s">
-        <v>258</v>
-      </c>
-      <c r="E32" s="108" t="s">
-        <v>263</v>
+      <c r="D32" s="127">
+        <v>21.6</v>
+      </c>
+      <c r="E32" s="141" t="s">
+        <v>296</v>
       </c>
       <c r="F32" s="108" t="s">
-        <v>263</v>
+        <v>297</v>
       </c>
       <c r="G32" s="108" t="s">
+        <v>297</v>
+      </c>
+      <c r="H32" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="H32" s="109" t="s">
+      <c r="I32" s="109" t="s">
         <v>157</v>
       </c>
-      <c r="I32" s="110"/>
       <c r="J32" s="110"/>
-      <c r="K32" s="109" t="s">
+      <c r="K32" s="110"/>
+      <c r="L32" s="109" t="s">
         <v>160</v>
       </c>
-      <c r="L32" s="108"/>
       <c r="M32" s="108"/>
       <c r="N32" s="108"/>
       <c r="O32" s="108"/>
-    </row>
-    <row r="33" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="P32" s="108"/>
+    </row>
+    <row r="33" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A33" s="107">
-        <v>28</v>
-      </c>
-      <c r="B33" s="107" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="107"/>
+      <c r="C33" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C33" s="127">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="D33" s="135" t="s">
-        <v>260</v>
-      </c>
-      <c r="E33" s="108" t="s">
-        <v>264</v>
+      <c r="D33" s="127">
+        <v>21.7</v>
+      </c>
+      <c r="E33" s="135" t="s">
+        <v>233</v>
       </c>
       <c r="F33" s="108" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G33" s="108" t="s">
+        <v>262</v>
+      </c>
+      <c r="H33" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="H33" s="109" t="s">
-        <v>265</v>
-      </c>
-      <c r="I33" s="110"/>
+      <c r="I33" s="109" t="s">
+        <v>157</v>
+      </c>
       <c r="J33" s="110"/>
-      <c r="K33" s="109" t="s">
+      <c r="K33" s="110"/>
+      <c r="L33" s="109" t="s">
         <v>160</v>
-      </c>
-      <c r="L33" s="108" t="s">
-        <v>266</v>
       </c>
       <c r="M33" s="108"/>
       <c r="N33" s="108"/>
       <c r="O33" s="108"/>
-    </row>
-    <row r="34" spans="1:15" s="163" customFormat="1" ht="12.75">
-      <c r="A34" s="155">
-        <v>29</v>
-      </c>
-      <c r="B34" s="155" t="s">
-        <v>322</v>
-      </c>
-      <c r="C34" s="156">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="D34" s="157" t="s">
+      <c r="P33" s="108"/>
+    </row>
+    <row r="34" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A34" s="107">
+        <v>30</v>
+      </c>
+      <c r="B34" s="107"/>
+      <c r="C34" s="107" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" s="127">
+        <v>21.8</v>
+      </c>
+      <c r="E34" s="135" t="s">
+        <v>258</v>
+      </c>
+      <c r="F34" s="108" t="s">
+        <v>263</v>
+      </c>
+      <c r="G34" s="108" t="s">
+        <v>263</v>
+      </c>
+      <c r="H34" s="108" t="s">
+        <v>176</v>
+      </c>
+      <c r="I34" s="109" t="s">
+        <v>157</v>
+      </c>
+      <c r="J34" s="110"/>
+      <c r="K34" s="110"/>
+      <c r="L34" s="109" t="s">
+        <v>160</v>
+      </c>
+      <c r="M34" s="108"/>
+      <c r="N34" s="108"/>
+      <c r="O34" s="108"/>
+      <c r="P34" s="108"/>
+    </row>
+    <row r="35" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A35" s="107">
+        <v>31</v>
+      </c>
+      <c r="B35" s="107"/>
+      <c r="C35" s="107" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="127">
+        <v>21.9</v>
+      </c>
+      <c r="E35" s="135" t="s">
+        <v>260</v>
+      </c>
+      <c r="F35" s="108" t="s">
+        <v>264</v>
+      </c>
+      <c r="G35" s="108" t="s">
+        <v>264</v>
+      </c>
+      <c r="H35" s="108" t="s">
+        <v>176</v>
+      </c>
+      <c r="I35" s="109" t="s">
+        <v>265</v>
+      </c>
+      <c r="J35" s="110"/>
+      <c r="K35" s="110"/>
+      <c r="L35" s="109" t="s">
+        <v>160</v>
+      </c>
+      <c r="M35" s="108" t="s">
+        <v>266</v>
+      </c>
+      <c r="N35" s="108"/>
+      <c r="O35" s="108"/>
+      <c r="P35" s="108"/>
+    </row>
+    <row r="36" spans="1:16" s="162" customFormat="1" ht="12.75">
+      <c r="A36" s="155">
+        <v>32</v>
+      </c>
+      <c r="B36" s="155">
+        <v>92</v>
+      </c>
+      <c r="C36" s="155" t="s">
+        <v>323</v>
+      </c>
+      <c r="D36" s="164">
+        <v>21.1</v>
+      </c>
+      <c r="E36" s="156" t="s">
         <v>320</v>
       </c>
-      <c r="E34" s="158" t="s">
+      <c r="F36" s="157" t="s">
         <v>321</v>
       </c>
-      <c r="F34" s="158" t="s">
+      <c r="G36" s="157" t="s">
         <v>321</v>
       </c>
-      <c r="G34" s="159" t="s">
+      <c r="H36" s="158" t="s">
         <v>176</v>
       </c>
-      <c r="H34" s="160" t="s">
+      <c r="I36" s="159" t="s">
         <v>157</v>
       </c>
-      <c r="I34" s="161"/>
-      <c r="J34" s="161"/>
-      <c r="K34" s="160" t="s">
+      <c r="J36" s="160"/>
+      <c r="K36" s="160"/>
+      <c r="L36" s="159" t="s">
         <v>160</v>
       </c>
-      <c r="L34" s="159"/>
-      <c r="M34" s="159"/>
-      <c r="N34" s="160"/>
-      <c r="O34" s="162"/>
-    </row>
-    <row r="35" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A35" s="107"/>
-      <c r="B35" s="107"/>
-      <c r="C35" s="107"/>
-      <c r="D35" s="119"/>
-      <c r="E35" s="120"/>
-      <c r="F35" s="108"/>
-      <c r="G35" s="108"/>
-      <c r="H35" s="109"/>
-      <c r="I35" s="110"/>
-      <c r="J35" s="110"/>
-      <c r="K35" s="109"/>
-      <c r="L35" s="108"/>
-      <c r="M35" s="108"/>
-      <c r="N35" s="109"/>
-      <c r="O35" s="108"/>
+      <c r="M36" s="158"/>
+      <c r="N36" s="158"/>
+      <c r="O36" s="159"/>
+      <c r="P36" s="161"/>
+    </row>
+    <row r="37" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A37" s="107"/>
+      <c r="B37" s="107"/>
+      <c r="C37" s="107"/>
+      <c r="D37" s="107"/>
+      <c r="E37" s="119"/>
+      <c r="F37" s="120"/>
+      <c r="G37" s="108"/>
+      <c r="H37" s="108"/>
+      <c r="I37" s="109"/>
+      <c r="J37" s="110"/>
+      <c r="K37" s="110"/>
+      <c r="L37" s="109"/>
+      <c r="M37" s="108"/>
+      <c r="N37" s="108"/>
+      <c r="O37" s="109"/>
+      <c r="P37" s="108"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:P36"/>
   <mergeCells count="5">
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G6 G8:G15 G18:G35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H6 H20:H37 H8:H17">
       <formula1>"Caption,Textbox,DateTimePicker,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid, Image,Link,Form,Frame,Menu,MenuItem,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7">
       <formula1>"Caption,Dropdownchecklist,Textbox,DateTimePicker,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid, Image,Link,Form,Frame,Menu,MenuItem,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G16:G17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H18:H19">
       <formula1>"Caption,Textbox,DateTimePicker, SpinNumeric,Table, Cell,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid,GridColumn,Image,Link,Form,Frame,Menu,MenuItem,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H15 H18:H35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I20:I37 I5:I17">
       <formula1>"Text, Number, DateTime, Boolean"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K15 K18:K35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L20:L37 L5:L17">
       <formula1>"I,O,I/O"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8571,7 +8693,7 @@
       </c>
       <c r="I1" s="57" t="str">
         <f>'Update History'!J1</f>
-        <v>Thị Phượng</v>
+        <v>Tấn Đạt</v>
       </c>
       <c r="J1" s="56"/>
     </row>
@@ -8603,7 +8725,7 @@
       </c>
       <c r="I2" s="57" t="str">
         <f>'Update History'!J2</f>
-        <v>25/03/2017</v>
+        <v>26/01/2018</v>
       </c>
       <c r="J2" s="57"/>
     </row>
@@ -9138,7 +9260,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="222" t="s">
+      <c r="A1" s="223" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="105"/>
@@ -9168,12 +9290,12 @@
       </c>
       <c r="J1" s="34" t="str">
         <f>'Update History'!J1</f>
-        <v>Thị Phượng</v>
+        <v>Tấn Đạt</v>
       </c>
       <c r="K1" s="46"/>
     </row>
     <row r="2" spans="1:11" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="223"/>
+      <c r="A2" s="224"/>
       <c r="B2" s="106"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
@@ -9201,7 +9323,7 @@
       </c>
       <c r="J2" s="34" t="str">
         <f>'Update History'!J2</f>
-        <v>25/03/2017</v>
+        <v>26/01/2018</v>
       </c>
       <c r="K2" s="46"/>
     </row>
@@ -9221,15 +9343,15 @@
       <c r="E4" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="196" t="s">
+      <c r="F4" s="197" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="196"/>
-      <c r="H4" s="196" t="s">
+      <c r="G4" s="197"/>
+      <c r="H4" s="197" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="196"/>
-      <c r="J4" s="196"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
     </row>
     <row r="5" spans="1:11" s="117" customFormat="1" ht="30.75" customHeight="1">
       <c r="A5" s="114">
@@ -9245,13 +9367,13 @@
       <c r="E5" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="224" t="s">
+      <c r="F5" s="225" t="s">
         <v>269</v>
       </c>
-      <c r="G5" s="225"/>
-      <c r="H5" s="225"/>
-      <c r="I5" s="226"/>
-      <c r="J5" s="224" t="s">
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="227"/>
+      <c r="J5" s="225" t="s">
         <v>267</v>
       </c>
     </row>
@@ -9269,11 +9391,11 @@
       <c r="E6" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="F6" s="227"/>
-      <c r="G6" s="228"/>
-      <c r="H6" s="228"/>
-      <c r="I6" s="229"/>
-      <c r="J6" s="227"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="229"/>
+      <c r="H6" s="229"/>
+      <c r="I6" s="230"/>
+      <c r="J6" s="228"/>
     </row>
     <row r="7" spans="1:11" s="117" customFormat="1" ht="45.75" customHeight="1">
       <c r="A7" s="114">
@@ -9289,12 +9411,12 @@
       <c r="E7" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="219" t="s">
+      <c r="F7" s="220" t="s">
         <v>270</v>
       </c>
-      <c r="G7" s="220"/>
-      <c r="H7" s="220"/>
-      <c r="I7" s="221"/>
+      <c r="G7" s="221"/>
+      <c r="H7" s="221"/>
+      <c r="I7" s="222"/>
       <c r="J7" s="116" t="s">
         <v>190</v>
       </c>
@@ -9313,12 +9435,12 @@
       <c r="E8" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="219" t="s">
+      <c r="F8" s="220" t="s">
         <v>239</v>
       </c>
-      <c r="G8" s="220"/>
-      <c r="H8" s="220"/>
-      <c r="I8" s="221"/>
+      <c r="G8" s="221"/>
+      <c r="H8" s="221"/>
+      <c r="I8" s="222"/>
       <c r="J8" s="116" t="s">
         <v>240</v>
       </c>
@@ -9337,12 +9459,12 @@
       <c r="E9" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="F9" s="219" t="s">
+      <c r="F9" s="220" t="s">
         <v>271</v>
       </c>
-      <c r="G9" s="220"/>
-      <c r="H9" s="220"/>
-      <c r="I9" s="221"/>
+      <c r="G9" s="221"/>
+      <c r="H9" s="221"/>
+      <c r="I9" s="222"/>
       <c r="J9" s="116" t="s">
         <v>241</v>
       </c>
@@ -9373,515 +9495,535 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1048216"/>
+  <dimension ref="A1:R1048216"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="D10" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="15" style="22" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="22" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" style="23" customWidth="1"/>
-    <col min="12" max="12" width="19" style="23" customWidth="1"/>
-    <col min="13" max="13" width="11" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="37" style="23" customWidth="1"/>
-    <col min="16" max="17" width="12.7109375" style="23" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="22" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="22"/>
+    <col min="2" max="2" width="11.5703125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="15" style="22" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="22" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" style="23" customWidth="1"/>
+    <col min="13" max="13" width="19" style="23" customWidth="1"/>
+    <col min="14" max="14" width="11" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37" style="23" customWidth="1"/>
+    <col min="17" max="18" width="12.7109375" style="23" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" style="22" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="196" t="s">
+    <row r="1" spans="1:18" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A1" s="197" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="30" t="s">
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="242" t="str">
+      <c r="G1" s="243" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="G1" s="242"/>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="243"/>
+      <c r="I1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="47" t="str">
+      <c r="J1" s="47" t="str">
         <f>'Update History'!F1</f>
         <v>CRMF2080</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="45" t="str">
+      <c r="L1" s="45" t="str">
         <f>'Update History'!H1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="230" t="str">
+      <c r="N1" s="231" t="str">
         <f>'Update History'!J1</f>
-        <v>Thị Phượng</v>
-      </c>
-      <c r="N1" s="231"/>
+        <v>Tấn Đạt</v>
+      </c>
       <c r="O1" s="232"/>
-      <c r="P1" s="46"/>
+      <c r="P1" s="233"/>
       <c r="Q1" s="46"/>
-    </row>
-    <row r="2" spans="1:17" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="30" t="s">
+      <c r="R1" s="46"/>
+    </row>
+    <row r="2" spans="1:18" s="25" customFormat="1" ht="12" customHeight="1">
+      <c r="A2" s="197"/>
+      <c r="B2" s="197"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="242" t="str">
+      <c r="G2" s="243" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT-CRM</v>
       </c>
-      <c r="G2" s="242"/>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="243"/>
+      <c r="I2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="47" t="str">
+      <c r="J2" s="47" t="str">
         <f>'Update History'!F2</f>
         <v>Danh mục yêu cầu</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="K2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="45" t="str">
+      <c r="L2" s="45" t="str">
         <f>'Update History'!H2</f>
         <v>25/03/2017</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="M2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="230" t="str">
+      <c r="N2" s="231" t="str">
         <f>'Update History'!J2</f>
-        <v>25/03/2017</v>
-      </c>
-      <c r="N2" s="231"/>
+        <v>26/01/2018</v>
+      </c>
       <c r="O2" s="232"/>
-      <c r="P2" s="46"/>
+      <c r="P2" s="233"/>
       <c r="Q2" s="46"/>
-    </row>
-    <row r="4" spans="1:17" s="23" customFormat="1" ht="12" customHeight="1">
+      <c r="R2" s="46"/>
+    </row>
+    <row r="4" spans="1:18" s="23" customFormat="1" ht="25.5" customHeight="1">
       <c r="A4" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="D4" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="E4" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="F4" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="G4" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="201" t="s">
+      <c r="H4" s="202" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="203"/>
-      <c r="I4" s="203"/>
-      <c r="J4" s="202"/>
-      <c r="K4" s="35" t="s">
+      <c r="I4" s="204"/>
+      <c r="J4" s="204"/>
+      <c r="K4" s="203"/>
+      <c r="L4" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="M4" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="58" t="s">
+      <c r="N4" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="N4" s="58" t="s">
+      <c r="O4" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="35" t="s">
+      <c r="P4" s="35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="25" customFormat="1" ht="51.75" customHeight="1">
+    <row r="5" spans="1:18" s="25" customFormat="1" ht="51.75" customHeight="1">
       <c r="A5" s="107">
         <v>1</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="107"/>
+      <c r="C5" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="128" t="s">
+      <c r="D5" s="128" t="s">
         <v>221</v>
       </c>
-      <c r="D5" s="129" t="s">
+      <c r="E5" s="129" t="s">
         <v>191</v>
       </c>
-      <c r="E5" s="129" t="s">
+      <c r="F5" s="129" t="s">
         <v>192</v>
       </c>
-      <c r="F5" s="130" t="s">
+      <c r="G5" s="130" t="s">
         <v>199</v>
       </c>
-      <c r="G5" s="236" t="s">
+      <c r="H5" s="237" t="s">
         <v>217</v>
       </c>
-      <c r="H5" s="237"/>
-      <c r="I5" s="237"/>
+      <c r="I5" s="238"/>
       <c r="J5" s="238"/>
-      <c r="K5" s="122" t="s">
+      <c r="K5" s="239"/>
+      <c r="L5" s="122" t="s">
         <v>198</v>
       </c>
-      <c r="L5" s="122" t="s">
+      <c r="M5" s="122" t="s">
         <v>205</v>
       </c>
-      <c r="M5" s="131" t="s">
+      <c r="N5" s="131" t="s">
         <v>181</v>
       </c>
-      <c r="N5" s="131" t="s">
+      <c r="O5" s="131" t="s">
         <v>193</v>
       </c>
-      <c r="O5" s="128" t="s">
+      <c r="P5" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="P5" s="46"/>
       <c r="Q5" s="46"/>
-    </row>
-    <row r="6" spans="1:17" s="25" customFormat="1" ht="51.75" customHeight="1">
+      <c r="R5" s="46"/>
+    </row>
+    <row r="6" spans="1:18" s="25" customFormat="1" ht="51.75" customHeight="1">
       <c r="A6" s="107">
         <v>2</v>
       </c>
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="107"/>
+      <c r="C6" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="D6" s="108" t="s">
         <v>276</v>
       </c>
-      <c r="D6" s="129" t="s">
+      <c r="E6" s="129" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="129" t="s">
+      <c r="F6" s="129" t="s">
         <v>192</v>
       </c>
-      <c r="F6" s="130" t="s">
+      <c r="G6" s="130" t="s">
         <v>201</v>
       </c>
-      <c r="G6" s="239" t="s">
+      <c r="H6" s="240" t="s">
         <v>219</v>
       </c>
-      <c r="H6" s="240"/>
-      <c r="I6" s="240"/>
+      <c r="I6" s="241"/>
       <c r="J6" s="241"/>
-      <c r="K6" s="122" t="s">
+      <c r="K6" s="242"/>
+      <c r="L6" s="122" t="s">
         <v>194</v>
       </c>
-      <c r="L6" s="122" t="s">
+      <c r="M6" s="122" t="s">
         <v>274</v>
       </c>
-      <c r="M6" s="67" t="s">
+      <c r="N6" s="67" t="s">
         <v>220</v>
       </c>
-      <c r="N6" s="131" t="s">
+      <c r="O6" s="131" t="s">
         <v>193</v>
       </c>
-      <c r="O6" s="67" t="s">
+      <c r="P6" s="67" t="s">
         <v>275</v>
       </c>
-      <c r="P6" s="46"/>
       <c r="Q6" s="46"/>
-    </row>
-    <row r="7" spans="1:17" s="25" customFormat="1" ht="51.75" customHeight="1">
+      <c r="R6" s="46"/>
+    </row>
+    <row r="7" spans="1:18" s="25" customFormat="1" ht="51.75" customHeight="1">
       <c r="A7" s="107">
         <v>3</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="107"/>
+      <c r="C7" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="108" t="s">
+      <c r="D7" s="108" t="s">
         <v>277</v>
       </c>
-      <c r="D7" s="129" t="s">
+      <c r="E7" s="129" t="s">
         <v>191</v>
       </c>
-      <c r="E7" s="129" t="s">
+      <c r="F7" s="129" t="s">
         <v>192</v>
       </c>
-      <c r="F7" s="130" t="s">
+      <c r="G7" s="130" t="s">
         <v>200</v>
       </c>
-      <c r="G7" s="239" t="s">
+      <c r="H7" s="240" t="s">
         <v>219</v>
       </c>
-      <c r="H7" s="240"/>
-      <c r="I7" s="240"/>
+      <c r="I7" s="241"/>
       <c r="J7" s="241"/>
-      <c r="K7" s="122" t="s">
+      <c r="K7" s="242"/>
+      <c r="L7" s="122" t="s">
         <v>194</v>
       </c>
-      <c r="L7" s="122" t="s">
+      <c r="M7" s="122" t="s">
         <v>242</v>
       </c>
-      <c r="M7" s="67" t="s">
+      <c r="N7" s="67" t="s">
         <v>220</v>
       </c>
-      <c r="N7" s="131" t="s">
+      <c r="O7" s="131" t="s">
         <v>193</v>
       </c>
-      <c r="O7" s="67" t="s">
+      <c r="P7" s="67" t="s">
         <v>278</v>
       </c>
-      <c r="P7" s="46"/>
       <c r="Q7" s="46"/>
-    </row>
-    <row r="8" spans="1:17" s="151" customFormat="1" ht="135">
+      <c r="R7" s="46"/>
+    </row>
+    <row r="8" spans="1:18" s="151" customFormat="1" ht="169.5" customHeight="1">
       <c r="A8" s="144">
         <v>5</v>
       </c>
-      <c r="B8" s="144" t="s">
+      <c r="B8" s="155">
+        <v>92</v>
+      </c>
+      <c r="C8" s="144" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="145"/>
-      <c r="D8" s="146" t="s">
+      <c r="D8" s="145"/>
+      <c r="E8" s="146" t="s">
         <v>191</v>
       </c>
-      <c r="E8" s="146" t="s">
+      <c r="F8" s="146" t="s">
         <v>195</v>
       </c>
-      <c r="F8" s="147" t="s">
+      <c r="G8" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="G8" s="233" t="s">
-        <v>323</v>
-      </c>
-      <c r="H8" s="234"/>
-      <c r="I8" s="234"/>
+      <c r="H8" s="234" t="s">
+        <v>327</v>
+      </c>
+      <c r="I8" s="235"/>
       <c r="J8" s="235"/>
-      <c r="K8" s="164" t="s">
-        <v>324</v>
-      </c>
-      <c r="L8" s="164" t="s">
-        <v>325</v>
-      </c>
-      <c r="M8" s="148" t="s">
+      <c r="K8" s="236"/>
+      <c r="L8" s="163" t="s">
+        <v>329</v>
+      </c>
+      <c r="M8" s="163" t="s">
+        <v>330</v>
+      </c>
+      <c r="N8" s="148" t="s">
         <v>222</v>
       </c>
-      <c r="N8" s="149" t="s">
+      <c r="O8" s="149" t="s">
         <v>196</v>
       </c>
-      <c r="O8" s="148" t="s">
+      <c r="P8" s="148" t="s">
         <v>223</v>
       </c>
-      <c r="P8" s="150"/>
       <c r="Q8" s="150"/>
-    </row>
-    <row r="9" spans="1:17" s="25" customFormat="1" ht="87.75" customHeight="1">
+      <c r="R8" s="150"/>
+    </row>
+    <row r="9" spans="1:18" s="25" customFormat="1" ht="87.75" customHeight="1">
       <c r="A9" s="107">
         <v>6</v>
       </c>
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="107"/>
+      <c r="C9" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="108"/>
-      <c r="D9" s="129" t="s">
+      <c r="D9" s="108"/>
+      <c r="E9" s="129" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="129" t="s">
+      <c r="F9" s="129" t="s">
         <v>195</v>
       </c>
-      <c r="F9" s="130" t="s">
+      <c r="G9" s="130" t="s">
         <v>203</v>
       </c>
-      <c r="G9" s="243" t="s">
+      <c r="H9" s="244" t="s">
         <v>273</v>
       </c>
-      <c r="H9" s="244"/>
-      <c r="I9" s="244"/>
+      <c r="I9" s="245"/>
       <c r="J9" s="245"/>
-      <c r="K9" s="132" t="s">
+      <c r="K9" s="246"/>
+      <c r="L9" s="132" t="s">
         <v>272</v>
       </c>
-      <c r="L9" s="132" t="s">
+      <c r="M9" s="132" t="s">
         <v>298</v>
       </c>
-      <c r="M9" s="67" t="s">
+      <c r="N9" s="67" t="s">
         <v>224</v>
       </c>
-      <c r="N9" s="131" t="s">
+      <c r="O9" s="131" t="s">
         <v>196</v>
       </c>
-      <c r="O9" s="67" t="s">
+      <c r="P9" s="67" t="s">
         <v>225</v>
       </c>
-      <c r="P9" s="46"/>
       <c r="Q9" s="46"/>
-    </row>
-    <row r="10" spans="1:17" s="25" customFormat="1" ht="135" customHeight="1">
+      <c r="R9" s="46"/>
+    </row>
+    <row r="10" spans="1:18" s="25" customFormat="1" ht="135" customHeight="1">
       <c r="A10" s="107">
         <v>10</v>
       </c>
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="155">
+        <v>92</v>
+      </c>
+      <c r="C10" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C10" s="108"/>
-      <c r="D10" s="129" t="s">
+      <c r="D10" s="108"/>
+      <c r="E10" s="129" t="s">
         <v>191</v>
       </c>
-      <c r="E10" s="129" t="s">
+      <c r="F10" s="129" t="s">
         <v>195</v>
       </c>
-      <c r="F10" s="130" t="s">
+      <c r="G10" s="130" t="s">
         <v>204</v>
       </c>
-      <c r="G10" s="233" t="s">
-        <v>326</v>
-      </c>
-      <c r="H10" s="234"/>
-      <c r="I10" s="234"/>
+      <c r="H10" s="234" t="s">
+        <v>331</v>
+      </c>
+      <c r="I10" s="235"/>
       <c r="J10" s="235"/>
-      <c r="K10" s="164" t="s">
-        <v>327</v>
-      </c>
-      <c r="L10" s="164" t="s">
-        <v>328</v>
-      </c>
-      <c r="M10" s="67"/>
-      <c r="N10" s="131" t="s">
+      <c r="K10" s="236"/>
+      <c r="L10" s="163" t="s">
+        <v>332</v>
+      </c>
+      <c r="M10" s="163" t="s">
+        <v>333</v>
+      </c>
+      <c r="N10" s="67"/>
+      <c r="O10" s="131" t="s">
         <v>196</v>
       </c>
-      <c r="O10" s="67" t="s">
+      <c r="P10" s="67" t="s">
         <v>228</v>
       </c>
-      <c r="P10" s="46"/>
       <c r="Q10" s="46"/>
-    </row>
-    <row r="11" spans="1:17" s="25" customFormat="1" ht="51.75" customHeight="1">
+      <c r="R10" s="46"/>
+    </row>
+    <row r="11" spans="1:18" s="25" customFormat="1" ht="51.75" customHeight="1">
       <c r="A11" s="107">
         <v>11</v>
       </c>
-      <c r="B11" s="107" t="s">
+      <c r="B11" s="107"/>
+      <c r="C11" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="108"/>
-      <c r="D11" s="129" t="s">
+      <c r="D11" s="108"/>
+      <c r="E11" s="129" t="s">
         <v>191</v>
       </c>
-      <c r="E11" s="129" t="s">
+      <c r="F11" s="129" t="s">
         <v>192</v>
       </c>
-      <c r="F11" s="130" t="s">
+      <c r="G11" s="130" t="s">
         <v>226</v>
       </c>
-      <c r="G11" s="236" t="s">
+      <c r="H11" s="237" t="s">
         <v>229</v>
       </c>
-      <c r="H11" s="237"/>
-      <c r="I11" s="237"/>
+      <c r="I11" s="238"/>
       <c r="J11" s="238"/>
-      <c r="K11" s="118" t="s">
+      <c r="K11" s="239"/>
+      <c r="L11" s="118" t="s">
         <v>198</v>
       </c>
-      <c r="L11" s="118" t="s">
+      <c r="M11" s="118" t="s">
         <v>205</v>
       </c>
-      <c r="M11" s="133"/>
-      <c r="N11" s="134" t="s">
+      <c r="N11" s="133"/>
+      <c r="O11" s="134" t="s">
         <v>193</v>
       </c>
-      <c r="O11" s="67" t="s">
+      <c r="P11" s="67" t="s">
         <v>230</v>
       </c>
-      <c r="P11" s="46"/>
       <c r="Q11" s="46"/>
-    </row>
-    <row r="12" spans="1:17" s="25" customFormat="1" ht="135" customHeight="1">
+      <c r="R11" s="46"/>
+    </row>
+    <row r="12" spans="1:18" s="25" customFormat="1" ht="135" customHeight="1">
       <c r="A12" s="107">
         <v>11</v>
       </c>
-      <c r="B12" s="107" t="s">
+      <c r="B12" s="155">
+        <v>92</v>
+      </c>
+      <c r="C12" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="C12" s="108"/>
-      <c r="D12" s="129" t="s">
+      <c r="D12" s="108"/>
+      <c r="E12" s="129" t="s">
         <v>191</v>
       </c>
-      <c r="E12" s="129" t="s">
+      <c r="F12" s="129" t="s">
         <v>192</v>
       </c>
-      <c r="F12" s="130" t="s">
+      <c r="G12" s="130" t="s">
         <v>227</v>
       </c>
-      <c r="G12" s="233" t="s">
-        <v>326</v>
-      </c>
-      <c r="H12" s="234"/>
-      <c r="I12" s="234"/>
+      <c r="H12" s="234" t="s">
+        <v>331</v>
+      </c>
+      <c r="I12" s="235"/>
       <c r="J12" s="235"/>
-      <c r="K12" s="164" t="s">
-        <v>329</v>
-      </c>
-      <c r="L12" s="164" t="s">
-        <v>328</v>
-      </c>
-      <c r="M12" s="67" t="s">
+      <c r="K12" s="236"/>
+      <c r="L12" s="163" t="s">
+        <v>332</v>
+      </c>
+      <c r="M12" s="163" t="s">
+        <v>333</v>
+      </c>
+      <c r="N12" s="67" t="s">
         <v>231</v>
       </c>
-      <c r="N12" s="134" t="s">
+      <c r="O12" s="134" t="s">
         <v>193</v>
       </c>
-      <c r="O12" s="126" t="s">
+      <c r="P12" s="126" t="s">
         <v>232</v>
       </c>
-      <c r="P12" s="46"/>
       <c r="Q12" s="46"/>
-    </row>
-    <row r="1048216" spans="13:13" ht="12" customHeight="1">
-      <c r="M1048216" s="63"/>
+      <c r="R12" s="46"/>
+    </row>
+    <row r="1048216" spans="14:14" ht="12" customHeight="1">
+      <c r="N1048216" s="63"/>
     </row>
   </sheetData>
   <dataConsolidate link="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H7:K7"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="M1048216:M1048576 M11 M5:M6"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D12">
+    <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="N1048216:N1048576 N11 N5:N6"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E12">
       <formula1>"Select,Insert,Update,Delete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F12">
       <formula1>"SQL Script, ID SQL, ID Store, ID Function, ID Trigger"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:N12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O12">
       <formula1>"Load,Click,Double Click,Change,Selected,KeyDown,KeyPress,Hover,Focus,LostFocus"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9900,8 +10042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A20" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="F55" sqref="F54:F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -9917,10 +10059,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="197" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
+      <c r="B1" s="197"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -9947,12 +10089,12 @@
       </c>
       <c r="J1" s="34" t="str">
         <f>'Update History'!J1</f>
-        <v>Thị Phượng</v>
+        <v>Tấn Đạt</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
+      <c r="A2" s="197"/>
+      <c r="B2" s="197"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -9979,7 +10121,7 @@
       </c>
       <c r="J2" s="34" t="str">
         <f>'Update History'!J2</f>
-        <v>25/03/2017</v>
+        <v>26/01/2018</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1">
@@ -10190,16 +10332,16 @@
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
       <c r="B21" s="39"/>
-      <c r="C21" s="246" t="s">
+      <c r="C21" s="247" t="s">
         <v>281</v>
       </c>
-      <c r="D21" s="247"/>
-      <c r="E21" s="247"/>
-      <c r="F21" s="247"/>
-      <c r="G21" s="247"/>
-      <c r="H21" s="247"/>
-      <c r="I21" s="247"/>
-      <c r="J21" s="247"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
+      <c r="I21" s="248"/>
+      <c r="J21" s="248"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="B22" s="39"/>
@@ -10364,16 +10506,16 @@
     <row r="36" spans="1:10" ht="28.5" customHeight="1">
       <c r="A36" s="61"/>
       <c r="B36" s="39"/>
-      <c r="C36" s="248" t="s">
+      <c r="C36" s="249" t="s">
         <v>236</v>
       </c>
-      <c r="D36" s="248"/>
-      <c r="E36" s="248"/>
-      <c r="F36" s="248"/>
-      <c r="G36" s="248"/>
-      <c r="H36" s="248"/>
-      <c r="I36" s="248"/>
-      <c r="J36" s="248"/>
+      <c r="D36" s="249"/>
+      <c r="E36" s="249"/>
+      <c r="F36" s="249"/>
+      <c r="G36" s="249"/>
+      <c r="H36" s="249"/>
+      <c r="I36" s="249"/>
+      <c r="J36" s="249"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="A37" s="38"/>
@@ -10501,13 +10643,13 @@
     </row>
     <row r="47" spans="1:10" ht="12" customHeight="1">
       <c r="B47" s="39"/>
-      <c r="C47" s="249"/>
-      <c r="D47" s="249"/>
-      <c r="E47" s="249"/>
-      <c r="F47" s="249"/>
-      <c r="G47" s="249"/>
-      <c r="H47" s="249"/>
-      <c r="I47" s="249"/>
+      <c r="C47" s="250"/>
+      <c r="D47" s="250"/>
+      <c r="E47" s="250"/>
+      <c r="F47" s="250"/>
+      <c r="G47" s="250"/>
+      <c r="H47" s="250"/>
+      <c r="I47" s="250"/>
       <c r="J47" s="42"/>
     </row>
     <row r="48" spans="1:10" ht="12" customHeight="1">
@@ -11150,10 +11292,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="197" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
+      <c r="B1" s="197"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -11180,12 +11322,12 @@
       </c>
       <c r="J1" s="34" t="str">
         <f>'Update History'!J1</f>
-        <v>Thị Phượng</v>
+        <v>Tấn Đạt</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
+      <c r="A2" s="197"/>
+      <c r="B2" s="197"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -11212,7 +11354,7 @@
       </c>
       <c r="J2" s="34" t="str">
         <f>'Update History'!J2</f>
-        <v>25/03/2017</v>
+        <v>26/01/2018</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1">

</xml_diff>